<commit_message>
Elements spreadsheet: cleaned first few cells.
</commit_message>
<xml_diff>
--- a/Elements.xlsx
+++ b/Elements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="505">
   <si>
     <t>Fl</t>
   </si>
@@ -135,6 +135,20 @@
   <si>
     <r>
       <t>4.002602(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>20.1797(6)</t>
     </r>
     <r>
       <rPr>
@@ -2274,8 +2288,123 @@
     <t>the Latin 'carbo', meaning charcoal</t>
   </si>
   <si>
-    <r>
-      <t>12.011</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Nitrogen</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the Greek 'nitron' and 'genes' meaning </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>nitre-forming</t>
+    </r>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Oxygen</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the Greek 'oxy' and 'genes' meaning </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>acid-forming</t>
+    </r>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Fluorine</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the Latin 'fluere', meaning </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>to flow</t>
+    </r>
+  </si>
+  <si>
+    <t>18.9984032(5)</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>Neon</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the Greek 'neos', meaning </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>new</t>
+    </r>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>Sodium</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the English word </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>soda</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>natrium</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> in Latin)</t>
     </r>
     <r>
       <rPr>
@@ -2283,14 +2412,93 @@
         <sz val="10"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t>[2]</t>
+    </r>
+  </si>
+  <si>
+    <t>22.98976928(2)</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>Magnesium</t>
+  </si>
+  <si>
+    <t>Magnesia, a district of Eastern Thessaly in Greece</t>
+  </si>
+  <si>
+    <t>Al</t>
+  </si>
+  <si>
+    <t>Aluminium</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the Latin name for alum, 'alumen' meaning </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>bitter salt</t>
+    </r>
+  </si>
+  <si>
+    <t>26.9815386(8)</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Silicon</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the Latin 'silex' or 'silicis', meaning </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>flint</t>
+    </r>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Phosphorus</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the Greek 'phosphoros', meaning </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>bringer of light</t>
+    </r>
+  </si>
+  <si>
+    <t>30.973762(2)</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Sulfur</t>
+  </si>
+  <si>
+    <r>
+      <t>Either from the Sanskrit 'sulvere', or the Latin 'sulfurium', both names for sulfur</t>
     </r>
     <r>
       <rPr>
@@ -2298,429 +2506,7 @@
         <sz val="10"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>9</t>
-    </r>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Nitrogen</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">the Greek 'nitron' and 'genes' meaning </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>nitre-forming</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>14.007</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>9</t>
-    </r>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Oxygen</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">the Greek 'oxy' and 'genes' meaning </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>acid-forming</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>15.999</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>9</t>
-    </r>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Fluorine</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">the Latin 'fluere', meaning </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>to flow</t>
-    </r>
-  </si>
-  <si>
-    <t>18.9984032(5)</t>
-  </si>
-  <si>
-    <t>Ne</t>
-  </si>
-  <si>
-    <t>Neon</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">the Greek 'neos', meaning </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>new</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>20.1797(6)</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
-    <t>Na</t>
-  </si>
-  <si>
-    <t>Sodium</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">the English word </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>soda</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>natrium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> in Latin)</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
       <t>[2]</t>
-    </r>
-  </si>
-  <si>
-    <t>22.98976928(2)</t>
-  </si>
-  <si>
-    <t>Mg</t>
-  </si>
-  <si>
-    <t>Magnesium</t>
-  </si>
-  <si>
-    <t>Magnesia, a district of Eastern Thessaly in Greece</t>
-  </si>
-  <si>
-    <t>Al</t>
-  </si>
-  <si>
-    <t>Aluminium</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">the Latin name for alum, 'alumen' meaning </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>bitter salt</t>
-    </r>
-  </si>
-  <si>
-    <t>26.9815386(8)</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>Silicon</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">the Latin 'silex' or 'silicis', meaning </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>flint</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>28.085</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>9</t>
-    </r>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Phosphorus</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">the Greek 'phosphoros', meaning </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>bringer of light</t>
-    </r>
-  </si>
-  <si>
-    <t>30.973762(2)</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Sulfur</t>
-  </si>
-  <si>
-    <r>
-      <t>Either from the Sanskrit 'sulvere', or the Latin 'sulfurium', both names for sulfur</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>[2]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>32.06</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t>9</t>
     </r>
   </si>
   <si>
@@ -3219,51 +3005,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:13" ht="26">
       <c r="A1" s="13" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15">
@@ -3274,23 +3060,23 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="L2" s="14"/>
       <c r="M2" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="78">
@@ -3298,13 +3084,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -3339,13 +3125,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E4" s="3">
         <v>18</v>
@@ -3369,7 +3155,7 @@
         <v>5.1929999999999996</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M4" s="3">
         <v>8.0000000000000002E-3</v>
@@ -3380,13 +3166,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -3421,13 +3207,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
@@ -3436,7 +3222,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="H6" s="3">
         <v>1.85</v>
@@ -3462,13 +3248,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E7" s="3">
         <v>13</v>
@@ -3503,13 +3289,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E8" s="3">
         <v>14</v>
@@ -3517,8 +3303,8 @@
       <c r="F8" s="3">
         <v>2</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>468</v>
+      <c r="G8" s="3">
+        <v>12.010999999999999</v>
       </c>
       <c r="H8" s="3">
         <v>2.2669999999999999</v>
@@ -3558,8 +3344,8 @@
       <c r="F9" s="3">
         <v>2</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>472</v>
+      <c r="G9" s="3">
+        <v>14.007</v>
       </c>
       <c r="H9" s="3">
         <v>1.2505999999999999E-3</v>
@@ -3585,13 +3371,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>474</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>475</v>
       </c>
       <c r="E10" s="3">
         <v>16</v>
@@ -3599,8 +3385,8 @@
       <c r="F10" s="3">
         <v>2</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>476</v>
+      <c r="G10" s="3">
+        <v>15.999000000000001</v>
       </c>
       <c r="H10" s="3">
         <v>1.4289999999999999E-3</v>
@@ -3626,13 +3412,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>477</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>479</v>
       </c>
       <c r="E11" s="3">
         <v>17</v>
@@ -3641,7 +3427,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H11" s="3">
         <v>1.696E-3</v>
@@ -3667,13 +3453,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>481</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>483</v>
       </c>
       <c r="E12" s="3">
         <v>18</v>
@@ -3682,7 +3468,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>484</v>
+        <v>30</v>
       </c>
       <c r="H12" s="3">
         <v>8.9990000000000003E-4</v>
@@ -3697,7 +3483,7 @@
         <v>1.03</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M12" s="3">
         <v>5.0000000000000001E-3</v>
@@ -3708,13 +3494,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -3723,7 +3509,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="H13" s="3">
         <v>0.97099999999999997</v>
@@ -3749,13 +3535,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E14" s="3">
         <v>2</v>
@@ -3763,8 +3549,8 @@
       <c r="F14" s="3">
         <v>3</v>
       </c>
-      <c r="G14" s="5">
-        <v>24.305900000000001</v>
+      <c r="G14">
+        <v>24.305</v>
       </c>
       <c r="H14" s="3">
         <v>1.738</v>
@@ -3790,13 +3576,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E15" s="3">
         <v>13</v>
@@ -3805,7 +3591,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="H15" s="3">
         <v>2.698</v>
@@ -3831,13 +3617,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E16" s="3">
         <v>14</v>
@@ -3845,8 +3631,8 @@
       <c r="F16" s="3">
         <v>3</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>499</v>
+      <c r="G16" s="3">
+        <v>28.085000000000001</v>
       </c>
       <c r="H16" s="3">
         <v>2.3296000000000001</v>
@@ -3872,13 +3658,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="E17" s="3">
         <v>15</v>
@@ -3887,7 +3673,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="H17" s="3">
         <v>1.82</v>
@@ -3913,13 +3699,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="E18" s="3">
         <v>16</v>
@@ -3927,8 +3713,8 @@
       <c r="F18" s="3">
         <v>3</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>507</v>
+      <c r="G18" s="3">
+        <v>32.06</v>
       </c>
       <c r="H18" s="3">
         <v>2.0670000000000002</v>
@@ -3954,13 +3740,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E19" s="3">
         <v>17</v>
@@ -3969,7 +3755,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H19" s="3">
         <v>3.2139999999999998E-3</v>
@@ -3995,13 +3781,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E20" s="3">
         <v>18</v>
@@ -4010,7 +3796,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H20" s="3">
         <v>1.7837E-3</v>
@@ -4025,7 +3811,7 @@
         <v>0.52</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M20" s="3">
         <v>3.5</v>
@@ -4036,13 +3822,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -4051,7 +3837,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H21" s="3">
         <v>0.86199999999999999</v>
@@ -4077,13 +3863,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E22" s="3">
         <v>2</v>
@@ -4092,7 +3878,7 @@
         <v>4</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H22" s="3">
         <v>1.54</v>
@@ -4118,13 +3904,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E23" s="3">
         <v>3</v>
@@ -4133,7 +3919,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H23" s="3">
         <v>2.9889999999999999</v>
@@ -4159,13 +3945,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E24" s="3">
         <v>4</v>
@@ -4174,7 +3960,7 @@
         <v>4</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="H24" s="3">
         <v>4.54</v>
@@ -4200,13 +3986,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E25" s="3">
         <v>5</v>
@@ -4215,7 +4001,7 @@
         <v>4</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H25" s="3">
         <v>6.11</v>
@@ -4241,13 +4027,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E26" s="3">
         <v>6</v>
@@ -4256,7 +4042,7 @@
         <v>4</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="H26" s="3">
         <v>7.15</v>
@@ -4282,13 +4068,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E27" s="3">
         <v>7</v>
@@ -4297,7 +4083,7 @@
         <v>4</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H27" s="3">
         <v>7.44</v>
@@ -4323,13 +4109,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E28" s="3">
         <v>8</v>
@@ -4338,7 +4124,7 @@
         <v>4</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="H28" s="3">
         <v>7.8739999999999997</v>
@@ -4364,13 +4150,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E29" s="3">
         <v>9</v>
@@ -4379,7 +4165,7 @@
         <v>4</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="H29" s="3">
         <v>8.86</v>
@@ -4405,13 +4191,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E30" s="3">
         <v>10</v>
@@ -4420,7 +4206,7 @@
         <v>4</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H30" s="3">
         <v>8.9120000000000008</v>
@@ -4446,13 +4232,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E31" s="3">
         <v>11</v>
@@ -4461,7 +4247,7 @@
         <v>4</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="H31" s="3">
         <v>8.9600000000000009</v>
@@ -4487,13 +4273,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E32" s="3">
         <v>12</v>
@@ -4502,7 +4288,7 @@
         <v>4</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="H32" s="3">
         <v>7.1340000000000003</v>
@@ -4528,13 +4314,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E33" s="3">
         <v>13</v>
@@ -4543,7 +4329,7 @@
         <v>4</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H33" s="3">
         <v>5.907</v>
@@ -4569,13 +4355,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E34" s="3">
         <v>14</v>
@@ -4584,7 +4370,7 @@
         <v>4</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H34" s="3">
         <v>5.3230000000000004</v>
@@ -4610,13 +4396,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E35" s="3">
         <v>15</v>
@@ -4625,13 +4411,13 @@
         <v>4</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H35" s="3">
         <v>5.7759999999999998</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="J35" s="3">
         <v>887</v>
@@ -4651,13 +4437,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E36" s="3">
         <v>16</v>
@@ -4666,7 +4452,7 @@
         <v>4</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H36" s="3">
         <v>4.8090000000000002</v>
@@ -4692,13 +4478,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E37" s="3">
         <v>17</v>
@@ -4733,13 +4519,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E38" s="3">
         <v>18</v>
@@ -4748,7 +4534,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H38" s="3">
         <v>3.7330000000000002E-3</v>
@@ -4766,7 +4552,7 @@
         <v>3</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="52">
@@ -4774,13 +4560,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E39" s="3">
         <v>1</v>
@@ -4789,7 +4575,7 @@
         <v>5</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H39" s="3">
         <v>1.532</v>
@@ -4815,13 +4601,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E40" s="3">
         <v>2</v>
@@ -4830,7 +4616,7 @@
         <v>5</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H40" s="3">
         <v>2.64</v>
@@ -4856,13 +4642,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E41" s="3">
         <v>3</v>
@@ -4871,7 +4657,7 @@
         <v>5</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H41" s="3">
         <v>4.4690000000000003</v>
@@ -4897,13 +4683,13 @@
         <v>40</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E42" s="3">
         <v>4</v>
@@ -4912,7 +4698,7 @@
         <v>5</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="H42" s="3">
         <v>6.5060000000000002</v>
@@ -4938,13 +4724,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E43" s="3">
         <v>5</v>
@@ -4953,7 +4739,7 @@
         <v>5</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H43" s="3">
         <v>8.57</v>
@@ -4979,13 +4765,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E44" s="3">
         <v>6</v>
@@ -4994,7 +4780,7 @@
         <v>5</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H44" s="3">
         <v>10.220000000000001</v>
@@ -5020,13 +4806,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E45" s="3">
         <v>7</v>
@@ -5035,7 +4821,7 @@
         <v>5</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H45" s="3">
         <v>11.5</v>
@@ -5047,13 +4833,13 @@
         <v>4538</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L45" s="3">
         <v>1.9</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="52">
@@ -5061,13 +4847,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E46" s="3">
         <v>8</v>
@@ -5076,7 +4862,7 @@
         <v>5</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="H46" s="3">
         <v>12.37</v>
@@ -5102,13 +4888,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E47" s="3">
         <v>9</v>
@@ -5117,7 +4903,7 @@
         <v>5</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H47" s="3">
         <v>12.41</v>
@@ -5143,13 +4929,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E48" s="3">
         <v>10</v>
@@ -5158,7 +4944,7 @@
         <v>5</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H48" s="3">
         <v>12.02</v>
@@ -5184,13 +4970,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E49" s="3">
         <v>11</v>
@@ -5199,7 +4985,7 @@
         <v>5</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H49" s="3">
         <v>10.500999999999999</v>
@@ -5225,13 +5011,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E50" s="3">
         <v>12</v>
@@ -5240,7 +5026,7 @@
         <v>5</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H50" s="3">
         <v>8.69</v>
@@ -5266,13 +5052,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E51" s="3">
         <v>13</v>
@@ -5281,7 +5067,7 @@
         <v>5</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H51" s="3">
         <v>7.31</v>
@@ -5307,13 +5093,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E52" s="3">
         <v>14</v>
@@ -5322,7 +5108,7 @@
         <v>5</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H52" s="3">
         <v>7.2869999999999999</v>
@@ -5348,13 +5134,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E53" s="3">
         <v>15</v>
@@ -5363,7 +5149,7 @@
         <v>5</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H53" s="3">
         <v>6.6849999999999996</v>
@@ -5389,13 +5175,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E54" s="3">
         <v>16</v>
@@ -5404,7 +5190,7 @@
         <v>5</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H54" s="3">
         <v>6.2320000000000002</v>
@@ -5430,13 +5216,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E55" s="3">
         <v>17</v>
@@ -5445,7 +5231,7 @@
         <v>5</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H55" s="3">
         <v>4.93</v>
@@ -5471,13 +5257,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E56" s="3">
         <v>18</v>
@@ -5486,7 +5272,7 @@
         <v>5</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H56" s="3">
         <v>5.8869999999999999E-3</v>
@@ -5504,7 +5290,7 @@
         <v>2.6</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="52">
@@ -5512,13 +5298,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E57" s="3">
         <v>1</v>
@@ -5527,7 +5313,7 @@
         <v>6</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H57" s="3">
         <v>1.873</v>
@@ -5553,13 +5339,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E58" s="3">
         <v>2</v>
@@ -5568,7 +5354,7 @@
         <v>6</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H58" s="3">
         <v>3.5939999999999999</v>
@@ -5594,20 +5380,20 @@
         <v>57</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3">
         <v>6</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H59" s="3">
         <v>6.1449999999999996</v>
@@ -5633,20 +5419,20 @@
         <v>58</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3">
         <v>6</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H60" s="3">
         <v>6.77</v>
@@ -5672,20 +5458,20 @@
         <v>59</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3">
         <v>6</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H61" s="3">
         <v>6.7729999999999997</v>
@@ -5711,20 +5497,20 @@
         <v>60</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3">
         <v>6</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H62" s="3">
         <v>7.0069999999999997</v>
@@ -5750,20 +5536,20 @@
         <v>61</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3">
         <v>6</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H63" s="3">
         <v>7.26</v>
@@ -5775,13 +5561,13 @@
         <v>3273</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L63" s="3">
         <v>1.1299999999999999</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="78">
@@ -5789,20 +5575,20 @@
         <v>62</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3">
         <v>6</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H64" s="3">
         <v>7.52</v>
@@ -5828,20 +5614,20 @@
         <v>63</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3">
         <v>6</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H65" s="3">
         <v>5.2430000000000003</v>
@@ -5867,20 +5653,20 @@
         <v>64</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3">
         <v>6</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H66" s="3">
         <v>7.8949999999999996</v>
@@ -5906,20 +5692,20 @@
         <v>65</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3">
         <v>6</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H67" s="3">
         <v>8.2289999999999992</v>
@@ -5945,20 +5731,20 @@
         <v>66</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3">
         <v>6</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H68" s="3">
         <v>8.5500000000000007</v>
@@ -5984,20 +5770,20 @@
         <v>67</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3">
         <v>6</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H69" s="3">
         <v>8.7949999999999999</v>
@@ -6023,20 +5809,20 @@
         <v>68</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3">
         <v>6</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H70" s="3">
         <v>9.0660000000000007</v>
@@ -6062,20 +5848,20 @@
         <v>69</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3">
         <v>6</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H71" s="3">
         <v>9.3209999999999997</v>
@@ -6101,20 +5887,20 @@
         <v>70</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3">
         <v>6</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H72" s="3">
         <v>6.9649999999999999</v>
@@ -6140,13 +5926,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E73" s="3">
         <v>3</v>
@@ -6155,7 +5941,7 @@
         <v>6</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H73" s="3">
         <v>9.84</v>
@@ -6181,13 +5967,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E74" s="3">
         <v>4</v>
@@ -6196,7 +5982,7 @@
         <v>6</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H74" s="3">
         <v>13.31</v>
@@ -6222,13 +6008,13 @@
         <v>73</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E75" s="3">
         <v>5</v>
@@ -6237,7 +6023,7 @@
         <v>6</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H75" s="3">
         <v>16.654</v>
@@ -6263,13 +6049,13 @@
         <v>74</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E76" s="3">
         <v>6</v>
@@ -6278,7 +6064,7 @@
         <v>6</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H76" s="3">
         <v>19.25</v>
@@ -6304,13 +6090,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E77" s="3">
         <v>7</v>
@@ -6319,7 +6105,7 @@
         <v>6</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H77" s="3">
         <v>21.02</v>
@@ -6337,7 +6123,7 @@
         <v>1.9</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="52">
@@ -6345,13 +6131,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E78" s="3">
         <v>8</v>
@@ -6360,7 +6146,7 @@
         <v>6</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H78" s="3">
         <v>22.61</v>
@@ -6386,13 +6172,13 @@
         <v>77</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E79" s="3">
         <v>9</v>
@@ -6401,7 +6187,7 @@
         <v>6</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H79" s="3">
         <v>22.56</v>
@@ -6427,13 +6213,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E80" s="3">
         <v>10</v>
@@ -6442,7 +6228,7 @@
         <v>6</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H80" s="3">
         <v>21.46</v>
@@ -6468,13 +6254,13 @@
         <v>79</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E81" s="3">
         <v>11</v>
@@ -6483,7 +6269,7 @@
         <v>6</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H81" s="3">
         <v>19.282</v>
@@ -6509,13 +6295,13 @@
         <v>80</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E82" s="3">
         <v>12</v>
@@ -6524,7 +6310,7 @@
         <v>6</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H82" s="3">
         <v>13.5336</v>
@@ -6550,13 +6336,13 @@
         <v>81</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E83" s="3">
         <v>13</v>
@@ -6591,13 +6377,13 @@
         <v>82</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E84" s="3">
         <v>14</v>
@@ -6606,7 +6392,7 @@
         <v>6</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H84" s="3">
         <v>11.342000000000001</v>
@@ -6632,13 +6418,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E85" s="3">
         <v>15</v>
@@ -6647,7 +6433,7 @@
         <v>6</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H85" s="3">
         <v>9.8070000000000004</v>
@@ -6673,13 +6459,13 @@
         <v>84</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E86" s="3">
         <v>16</v>
@@ -6688,7 +6474,7 @@
         <v>6</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H86" s="3">
         <v>9.32</v>
@@ -6700,13 +6486,13 @@
         <v>1235</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L86" s="3">
         <v>2</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="52">
@@ -6714,13 +6500,13 @@
         <v>85</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E87" s="3">
         <v>17</v>
@@ -6729,7 +6515,7 @@
         <v>6</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H87" s="3">
         <v>7</v>
@@ -6741,13 +6527,13 @@
         <v>610</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L87" s="3">
         <v>2.2000000000000002</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="117">
@@ -6755,13 +6541,13 @@
         <v>86</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E88" s="3">
         <v>18</v>
@@ -6770,7 +6556,7 @@
         <v>6</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H88" s="3">
         <v>9.7300000000000008E-3</v>
@@ -6788,7 +6574,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="52">
@@ -6796,13 +6582,13 @@
         <v>87</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E89" s="3">
         <v>1</v>
@@ -6811,7 +6597,7 @@
         <v>7</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H89" s="3">
         <v>1.87</v>
@@ -6823,13 +6609,13 @@
         <v>950</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L89" s="3">
         <v>0.7</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="39">
@@ -6837,13 +6623,13 @@
         <v>88</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E90" s="3">
         <v>2</v>
@@ -6852,7 +6638,7 @@
         <v>7</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H90" s="3">
         <v>5.5</v>
@@ -6870,7 +6656,7 @@
         <v>0.9</v>
       </c>
       <c r="M90" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="52">
@@ -6878,20 +6664,20 @@
         <v>89</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="3">
         <v>7</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H91" s="3">
         <v>10.07</v>
@@ -6909,7 +6695,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="52">
@@ -6917,20 +6703,20 @@
         <v>90</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3">
         <v>7</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H92" s="3">
         <v>11.72</v>
@@ -6956,20 +6742,20 @@
         <v>91</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3">
         <v>7</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H93" s="3">
         <v>15.37</v>
@@ -6981,13 +6767,13 @@
         <v>4300</v>
       </c>
       <c r="K93" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L93" s="3">
         <v>1.5</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="52">
@@ -6995,20 +6781,20 @@
         <v>92</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3">
         <v>7</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H94" s="3">
         <v>18.95</v>
@@ -7034,20 +6820,20 @@
         <v>93</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3">
         <v>7</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H95" s="3">
         <v>20.45</v>
@@ -7059,13 +6845,13 @@
         <v>4273</v>
       </c>
       <c r="K95" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L95" s="3">
         <v>1.36</v>
       </c>
       <c r="M95" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="52">
@@ -7073,20 +6859,20 @@
         <v>94</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3">
         <v>7</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H96" s="3">
         <v>19.84</v>
@@ -7098,13 +6884,13 @@
         <v>3501</v>
       </c>
       <c r="K96" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L96" s="3">
         <v>1.28</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="97" spans="1:13" ht="78">
@@ -7112,20 +6898,20 @@
         <v>95</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="3">
         <v>7</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H97" s="3">
         <v>13.69</v>
@@ -7137,13 +6923,13 @@
         <v>2880</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L97" s="3">
         <v>1.1299999999999999</v>
       </c>
       <c r="M97" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="98" spans="1:13" ht="78">
@@ -7151,20 +6937,20 @@
         <v>96</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3">
         <v>7</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H98" s="3">
         <v>13.51</v>
@@ -7176,13 +6962,13 @@
         <v>3383</v>
       </c>
       <c r="K98" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L98" s="3">
         <v>1.28</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="78">
@@ -7190,20 +6976,20 @@
         <v>97</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3">
         <v>7</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H99" s="3">
         <v>14.79</v>
@@ -7215,13 +7001,13 @@
         <v>2900</v>
       </c>
       <c r="K99" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L99" s="3">
         <v>1.3</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="78">
@@ -7229,20 +7015,20 @@
         <v>98</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3">
         <v>7</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H100" s="3">
         <v>15.1</v>
@@ -7251,16 +7037,16 @@
         <v>1173</v>
       </c>
       <c r="J100" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K100" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L100" s="3">
         <v>1.3</v>
       </c>
       <c r="M100" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="101" spans="1:13" ht="39">
@@ -7268,20 +7054,20 @@
         <v>99</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3">
         <v>7</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H101" s="3">
         <v>8.84</v>
@@ -7290,16 +7076,16 @@
         <v>1133</v>
       </c>
       <c r="J101" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L101" s="3">
         <v>1.3</v>
       </c>
       <c r="M101" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="26">
@@ -7307,38 +7093,38 @@
         <v>100</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E102" s="3"/>
       <c r="F102" s="3">
         <v>7</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I102" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K102" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L102" s="3">
         <v>1.3</v>
       </c>
       <c r="M102" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="52">
@@ -7346,38 +7132,38 @@
         <v>101</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E103" s="3"/>
       <c r="F103" s="3">
         <v>7</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I103" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K103" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L103" s="3">
         <v>1.3</v>
       </c>
       <c r="M103" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="104">
@@ -7385,38 +7171,38 @@
         <v>102</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3">
         <v>7</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I104" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K104" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L104" s="3">
         <v>1.3</v>
       </c>
       <c r="M104" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="105" spans="1:13" ht="39">
@@ -7424,13 +7210,13 @@
         <v>103</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E105" s="3">
         <v>3</v>
@@ -7439,25 +7225,25 @@
         <v>7</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I105" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K105" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L105" s="3">
         <v>1.3</v>
       </c>
       <c r="M105" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="1:13" ht="52">
@@ -7465,13 +7251,13 @@
         <v>104</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E106" s="3">
         <v>4</v>
@@ -7480,25 +7266,25 @@
         <v>7</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I106" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J106" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L106" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M106" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="26">
@@ -7506,13 +7292,13 @@
         <v>105</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E107" s="3">
         <v>5</v>
@@ -7521,25 +7307,25 @@
         <v>7</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L107" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M107" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="108" spans="1:13" ht="39">
@@ -7547,13 +7333,13 @@
         <v>106</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E108" s="3">
         <v>6</v>
@@ -7562,25 +7348,25 @@
         <v>7</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K108" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L108" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M108" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="109" spans="1:13" ht="26">
@@ -7588,13 +7374,13 @@
         <v>107</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E109" s="3">
         <v>7</v>
@@ -7603,25 +7389,25 @@
         <v>7</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H109" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L109" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M109" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="110" spans="1:13" ht="78">
@@ -7629,13 +7415,13 @@
         <v>108</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E110" s="3">
         <v>8</v>
@@ -7644,25 +7430,25 @@
         <v>7</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K110" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L110" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M110" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="111" spans="1:13" ht="26">
@@ -7670,13 +7456,13 @@
         <v>109</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E111" s="3">
         <v>9</v>
@@ -7685,25 +7471,25 @@
         <v>7</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J111" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K111" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L111" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M111" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="112" spans="1:13" ht="78">
@@ -7711,13 +7497,13 @@
         <v>110</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E112" s="3">
         <v>10</v>
@@ -7726,25 +7512,25 @@
         <v>7</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H112" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K112" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L112" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M112" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="113" spans="1:13" ht="52">
@@ -7752,13 +7538,13 @@
         <v>111</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E113" s="3">
         <v>11</v>
@@ -7767,25 +7553,25 @@
         <v>7</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J113" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K113" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L113" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M113" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="114" spans="1:13" ht="39">
@@ -7793,13 +7579,13 @@
         <v>112</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E114" s="3">
         <v>12</v>
@@ -7808,25 +7594,25 @@
         <v>7</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J114" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L114" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M114" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="115" spans="1:13" ht="52">
@@ -7834,13 +7620,13 @@
         <v>113</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E115" s="3">
         <v>13</v>
@@ -7849,25 +7635,25 @@
         <v>7</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I115" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L115" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M115" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="116" spans="1:13" ht="39">
@@ -7902,13 +7688,13 @@
         <v>6</v>
       </c>
       <c r="K116" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L116" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M116" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="117" spans="1:13" ht="52">
@@ -7922,7 +7708,7 @@
         <v>8</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E117" s="3">
         <v>15</v>
@@ -7937,19 +7723,19 @@
         <v>10</v>
       </c>
       <c r="I117" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J117" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K117" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L117" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M117" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="118" spans="1:13" ht="143">
@@ -7984,13 +7770,13 @@
         <v>17</v>
       </c>
       <c r="K118" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L118" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M118" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="119" spans="1:13" ht="52">
@@ -8004,7 +7790,7 @@
         <v>19</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E119" s="3">
         <v>17</v>
@@ -8025,13 +7811,13 @@
         <v>23</v>
       </c>
       <c r="K119" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L119" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M119" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="120" spans="1:13" ht="52">
@@ -8045,7 +7831,7 @@
         <v>25</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E120" s="3">
         <v>18</v>
@@ -8066,17 +7852,16 @@
         <v>28</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L120" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M120" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="7">
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
@@ -8118,281 +7903,280 @@
     <hyperlink ref="C12" r:id="rId28" tooltip="Neon"/>
     <hyperlink ref="C13" r:id="rId29" tooltip="Sodium"/>
     <hyperlink ref="C14" r:id="rId30" tooltip="Magnesium"/>
-    <hyperlink ref="G14" r:id="rId31" location="endnote_9" display="https://en.wikipedia.org/wiki/List_of_elements - endnote_9"/>
-    <hyperlink ref="C15" r:id="rId32" tooltip="Aluminium"/>
-    <hyperlink ref="C16" r:id="rId33" tooltip="Silicon"/>
-    <hyperlink ref="C17" r:id="rId34" tooltip="Phosphorus"/>
-    <hyperlink ref="C18" r:id="rId35" tooltip="Sulfur"/>
-    <hyperlink ref="C19" r:id="rId36" tooltip="Chlorine"/>
-    <hyperlink ref="C20" r:id="rId37" tooltip="Argon"/>
-    <hyperlink ref="C21" r:id="rId38" tooltip="Potassium"/>
-    <hyperlink ref="D21" r:id="rId39" location="cite_note-innvista-2"/>
-    <hyperlink ref="C22" r:id="rId40" tooltip="Calcium"/>
-    <hyperlink ref="G22" r:id="rId41" location="endnote_2"/>
-    <hyperlink ref="C23" r:id="rId42" tooltip="Scandium"/>
-    <hyperlink ref="D23" r:id="rId43" tooltip="Scandinavia"/>
-    <hyperlink ref="C24" r:id="rId44" tooltip="Titanium"/>
-    <hyperlink ref="D24" r:id="rId45" tooltip="Titan (mythology)"/>
-    <hyperlink ref="C25" r:id="rId46" tooltip="Vanadium"/>
-    <hyperlink ref="C26" r:id="rId47" tooltip="Chromium"/>
-    <hyperlink ref="C27" r:id="rId48" tooltip="Manganese"/>
-    <hyperlink ref="C28" r:id="rId49" tooltip="Iron"/>
-    <hyperlink ref="D28" r:id="rId50" tooltip="Anglo-Saxon"/>
-    <hyperlink ref="C29" r:id="rId51" tooltip="Cobalt"/>
-    <hyperlink ref="D29" r:id="rId52" tooltip="German language"/>
-    <hyperlink ref="C30" r:id="rId53" tooltip="Nickel"/>
-    <hyperlink ref="C31" r:id="rId54" tooltip="Copper"/>
-    <hyperlink ref="D31" r:id="rId55" tooltip="Cyprus"/>
-    <hyperlink ref="G31" r:id="rId56" location="endnote_4"/>
-    <hyperlink ref="C32" r:id="rId57" tooltip="Zinc"/>
-    <hyperlink ref="D32" r:id="rId58" tooltip="Persian language"/>
-    <hyperlink ref="C33" r:id="rId59" tooltip="Gallium"/>
-    <hyperlink ref="D33" r:id="rId60" tooltip="France"/>
-    <hyperlink ref="C34" r:id="rId61" tooltip="Germanium"/>
-    <hyperlink ref="D34" r:id="rId62" tooltip="Germany"/>
-    <hyperlink ref="C35" r:id="rId63" tooltip="Arsenic"/>
-    <hyperlink ref="D35" r:id="rId64" tooltip="Orpiment"/>
-    <hyperlink ref="I35" r:id="rId65" location="endnote_7"/>
-    <hyperlink ref="C36" r:id="rId66" tooltip="Selenium"/>
-    <hyperlink ref="D36" r:id="rId67" tooltip="Moon"/>
-    <hyperlink ref="G36" r:id="rId68" location="endnote_4"/>
-    <hyperlink ref="C37" r:id="rId69" tooltip="Bromine"/>
-    <hyperlink ref="G37" r:id="rId70" location="endnote_9" display="https://en.wikipedia.org/wiki/List_of_elements - endnote_9"/>
-    <hyperlink ref="C38" r:id="rId71" tooltip="Krypton"/>
-    <hyperlink ref="C39" r:id="rId72" tooltip="Rubidium"/>
-    <hyperlink ref="G39" r:id="rId73" location="endnote_2"/>
-    <hyperlink ref="C40" r:id="rId74" tooltip="Strontium"/>
-    <hyperlink ref="C41" r:id="rId75" tooltip="Yttrium"/>
-    <hyperlink ref="C42" r:id="rId76" tooltip="Zirconium"/>
-    <hyperlink ref="G42" r:id="rId77" location="endnote_2"/>
-    <hyperlink ref="C43" r:id="rId78" tooltip="Niobium"/>
-    <hyperlink ref="C44" r:id="rId79" tooltip="Molybdenum"/>
-    <hyperlink ref="G44" r:id="rId80" location="endnote_2"/>
-    <hyperlink ref="C45" r:id="rId81" tooltip="Technetium"/>
-    <hyperlink ref="G45" r:id="rId82" location="endnote_1"/>
-    <hyperlink ref="C46" r:id="rId83" tooltip="Ruthenium"/>
-    <hyperlink ref="D46" r:id="rId84" tooltip="Russia"/>
-    <hyperlink ref="G46" r:id="rId85" location="endnote_2"/>
-    <hyperlink ref="C47" r:id="rId86" tooltip="Rhodium"/>
-    <hyperlink ref="C48" r:id="rId87" tooltip="Palladium"/>
-    <hyperlink ref="D48" r:id="rId88" tooltip="2 Pallas"/>
-    <hyperlink ref="G48" r:id="rId89" location="endnote_2"/>
-    <hyperlink ref="C49" r:id="rId90" tooltip="Silver"/>
-    <hyperlink ref="G49" r:id="rId91" location="endnote_2"/>
-    <hyperlink ref="C50" r:id="rId92" tooltip="Cadmium"/>
-    <hyperlink ref="G50" r:id="rId93" location="endnote_2"/>
-    <hyperlink ref="C51" r:id="rId94" tooltip="Indium"/>
-    <hyperlink ref="C52" r:id="rId95" tooltip="Tin"/>
-    <hyperlink ref="G52" r:id="rId96" location="endnote_2"/>
-    <hyperlink ref="C53" r:id="rId97" tooltip="Antimony"/>
-    <hyperlink ref="G53" r:id="rId98" location="endnote_2"/>
-    <hyperlink ref="C54" r:id="rId99" tooltip="Tellurium"/>
-    <hyperlink ref="G54" r:id="rId100" location="endnote_2"/>
-    <hyperlink ref="C55" r:id="rId101" tooltip="Iodine"/>
-    <hyperlink ref="C56" r:id="rId102" tooltip="Xenon"/>
-    <hyperlink ref="C57" r:id="rId103" tooltip="Caesium"/>
-    <hyperlink ref="C58" r:id="rId104" tooltip="Barium"/>
-    <hyperlink ref="C59" r:id="rId105" tooltip="Lanthanum"/>
-    <hyperlink ref="G59" r:id="rId106" location="endnote_2"/>
-    <hyperlink ref="C60" r:id="rId107" tooltip="Cerium"/>
-    <hyperlink ref="G60" r:id="rId108" location="endnote_2"/>
-    <hyperlink ref="C61" r:id="rId109" tooltip="Praseodymium"/>
-    <hyperlink ref="C62" r:id="rId110" tooltip="Neodymium"/>
-    <hyperlink ref="G62" r:id="rId111" location="endnote_2"/>
-    <hyperlink ref="C63" r:id="rId112" tooltip="Promethium"/>
-    <hyperlink ref="D63" r:id="rId113" tooltip="Prometheus"/>
-    <hyperlink ref="G63" r:id="rId114" location="endnote_1"/>
-    <hyperlink ref="C64" r:id="rId115" tooltip="Samarium"/>
-    <hyperlink ref="D64" r:id="rId116" tooltip="Samarskite"/>
-    <hyperlink ref="G64" r:id="rId117" location="endnote_2"/>
-    <hyperlink ref="C65" r:id="rId118" tooltip="Europium"/>
-    <hyperlink ref="D65" r:id="rId119" tooltip="Europe"/>
-    <hyperlink ref="G65" r:id="rId120" location="endnote_2"/>
-    <hyperlink ref="C66" r:id="rId121" tooltip="Gadolinium"/>
-    <hyperlink ref="D66" r:id="rId122" tooltip="Johan Gadolin"/>
-    <hyperlink ref="G66" r:id="rId123" location="endnote_2"/>
-    <hyperlink ref="C67" r:id="rId124" tooltip="Terbium"/>
-    <hyperlink ref="C68" r:id="rId125" tooltip="Dysprosium"/>
-    <hyperlink ref="G68" r:id="rId126" location="endnote_2"/>
-    <hyperlink ref="C69" r:id="rId127" tooltip="Holmium"/>
-    <hyperlink ref="D69" r:id="rId128" tooltip="Stockholm"/>
-    <hyperlink ref="C70" r:id="rId129" tooltip="Erbium"/>
-    <hyperlink ref="G70" r:id="rId130" location="endnote_2"/>
-    <hyperlink ref="C71" r:id="rId131" tooltip="Thulium"/>
-    <hyperlink ref="D71" r:id="rId132" tooltip="Thule"/>
-    <hyperlink ref="C72" r:id="rId133" tooltip="Ytterbium"/>
-    <hyperlink ref="G72" r:id="rId134" location="endnote_2"/>
-    <hyperlink ref="C73" r:id="rId135" tooltip="Lutetium"/>
-    <hyperlink ref="D73" r:id="rId136" tooltip="Paris"/>
-    <hyperlink ref="G73" r:id="rId137" location="endnote_2"/>
-    <hyperlink ref="C74" r:id="rId138" tooltip="Hafnium"/>
-    <hyperlink ref="D74" r:id="rId139" tooltip="Copenhagen"/>
-    <hyperlink ref="C75" r:id="rId140" tooltip="Tantalum"/>
-    <hyperlink ref="D75" r:id="rId141" tooltip="Tantalus"/>
-    <hyperlink ref="C76" r:id="rId142" tooltip="Tungsten"/>
-    <hyperlink ref="D76" r:id="rId143" location="cite_note-innvista-2"/>
-    <hyperlink ref="C77" r:id="rId144" tooltip="Rhenium"/>
-    <hyperlink ref="C78" r:id="rId145" tooltip="Osmium"/>
-    <hyperlink ref="G78" r:id="rId146" location="endnote_2"/>
-    <hyperlink ref="C79" r:id="rId147" tooltip="Iridium"/>
-    <hyperlink ref="D79" r:id="rId148" tooltip="Iris (mythology)"/>
-    <hyperlink ref="C80" r:id="rId149" tooltip="Platinum"/>
-    <hyperlink ref="D80" r:id="rId150" tooltip="Spanish language"/>
-    <hyperlink ref="C81" r:id="rId151" tooltip="Gold"/>
-    <hyperlink ref="D81" r:id="rId152" location="cite_note-innvista-2"/>
-    <hyperlink ref="C82" r:id="rId153" tooltip="Mercury (element)"/>
-    <hyperlink ref="C83" r:id="rId154" tooltip="Thallium"/>
-    <hyperlink ref="G83" r:id="rId155" location="endnote_9" display="https://en.wikipedia.org/wiki/List_of_elements - endnote_9"/>
-    <hyperlink ref="C84" r:id="rId156" tooltip="Lead"/>
-    <hyperlink ref="D84" r:id="rId157" location="cite_note-innvista-2"/>
-    <hyperlink ref="C85" r:id="rId158" tooltip="Bismuth"/>
-    <hyperlink ref="G85" r:id="rId159" location="endnote_1"/>
-    <hyperlink ref="C86" r:id="rId160" tooltip="Polonium"/>
-    <hyperlink ref="G86" r:id="rId161" location="endnote_1"/>
-    <hyperlink ref="C87" r:id="rId162" tooltip="Astatine"/>
-    <hyperlink ref="G87" r:id="rId163" location="endnote_1"/>
-    <hyperlink ref="C88" r:id="rId164" tooltip="Radon"/>
-    <hyperlink ref="G88" r:id="rId165" location="endnote_1"/>
-    <hyperlink ref="C89" r:id="rId166" tooltip="Francium"/>
-    <hyperlink ref="G89" r:id="rId167" location="endnote_1"/>
-    <hyperlink ref="C90" r:id="rId168" tooltip="Radium"/>
-    <hyperlink ref="G90" r:id="rId169" location="endnote_1"/>
-    <hyperlink ref="C91" r:id="rId170" tooltip="Actinium"/>
-    <hyperlink ref="G91" r:id="rId171" location="endnote_1"/>
-    <hyperlink ref="C92" r:id="rId172" tooltip="Thorium"/>
-    <hyperlink ref="D92" r:id="rId173" tooltip="Thor"/>
-    <hyperlink ref="C93" r:id="rId174" tooltip="Protactinium"/>
-    <hyperlink ref="G93" r:id="rId175" location="endnote_1"/>
-    <hyperlink ref="C94" r:id="rId176" tooltip="Uranium"/>
-    <hyperlink ref="D94" r:id="rId177" tooltip="Uranus"/>
-    <hyperlink ref="G94" r:id="rId178" location="endnote_1"/>
-    <hyperlink ref="C95" r:id="rId179" tooltip="Neptunium"/>
-    <hyperlink ref="D95" r:id="rId180" tooltip="Neptune"/>
-    <hyperlink ref="G95" r:id="rId181" location="endnote_1"/>
-    <hyperlink ref="C96" r:id="rId182" tooltip="Plutonium"/>
-    <hyperlink ref="D96" r:id="rId183" tooltip="Pluto"/>
-    <hyperlink ref="G96" r:id="rId184" location="endnote_1"/>
-    <hyperlink ref="C97" r:id="rId185" tooltip="Americium"/>
-    <hyperlink ref="D97" r:id="rId186" tooltip="Americas"/>
-    <hyperlink ref="G97" r:id="rId187" location="endnote_1"/>
-    <hyperlink ref="C98" r:id="rId188" tooltip="Curium"/>
-    <hyperlink ref="G98" r:id="rId189" location="endnote_1"/>
-    <hyperlink ref="C99" r:id="rId190" tooltip="Berkelium"/>
-    <hyperlink ref="D99" r:id="rId191" tooltip="Berkeley, California"/>
-    <hyperlink ref="G99" r:id="rId192" location="endnote_1"/>
-    <hyperlink ref="C100" r:id="rId193" tooltip="Californium"/>
-    <hyperlink ref="D100" r:id="rId194" tooltip="State of California"/>
-    <hyperlink ref="G100" r:id="rId195" location="endnote_1"/>
-    <hyperlink ref="J100" r:id="rId196" location="endnote_11"/>
-    <hyperlink ref="C101" r:id="rId197" tooltip="Einsteinium"/>
-    <hyperlink ref="D101" r:id="rId198" tooltip="Albert Einstein"/>
-    <hyperlink ref="G101" r:id="rId199" location="endnote_1"/>
-    <hyperlink ref="J101" r:id="rId200" location="endnote_11"/>
-    <hyperlink ref="M101" r:id="rId201" location="endnote_8"/>
-    <hyperlink ref="C102" r:id="rId202" tooltip="Fermium"/>
-    <hyperlink ref="D102" r:id="rId203" tooltip="Enrico Fermi"/>
-    <hyperlink ref="G102" r:id="rId204" location="endnote_1"/>
-    <hyperlink ref="I102" r:id="rId205" location="endnote_11"/>
-    <hyperlink ref="M102" r:id="rId206" location="endnote_8"/>
-    <hyperlink ref="C103" r:id="rId207" tooltip="Mendelevium"/>
-    <hyperlink ref="D103" r:id="rId208" tooltip="Dmitri Mendeleyev"/>
-    <hyperlink ref="G103" r:id="rId209" location="endnote_1"/>
-    <hyperlink ref="I103" r:id="rId210" location="endnote_11"/>
-    <hyperlink ref="M103" r:id="rId211" location="endnote_8"/>
-    <hyperlink ref="C104" r:id="rId212" tooltip="Nobelium"/>
-    <hyperlink ref="D104" r:id="rId213" tooltip="Alfred Nobel"/>
-    <hyperlink ref="G104" r:id="rId214" location="endnote_1"/>
-    <hyperlink ref="I104" r:id="rId215" location="endnote_11"/>
-    <hyperlink ref="M104" r:id="rId216" location="endnote_8"/>
-    <hyperlink ref="C105" r:id="rId217" tooltip="Lawrencium"/>
-    <hyperlink ref="D105" r:id="rId218" tooltip="Ernest O. Lawrence"/>
-    <hyperlink ref="G105" r:id="rId219" location="endnote_1"/>
-    <hyperlink ref="I105" r:id="rId220" location="endnote_11"/>
-    <hyperlink ref="M105" r:id="rId221" location="endnote_8"/>
-    <hyperlink ref="C106" r:id="rId222" tooltip="Rutherfordium"/>
-    <hyperlink ref="D106" r:id="rId223" tooltip="Ernest Rutherford"/>
-    <hyperlink ref="G106" r:id="rId224" location="endnote_1"/>
-    <hyperlink ref="H106" r:id="rId225" location="endnote_11"/>
-    <hyperlink ref="I106" r:id="rId226" location="endnote_11"/>
-    <hyperlink ref="J106" r:id="rId227" location="endnote_11"/>
-    <hyperlink ref="M106" r:id="rId228" location="endnote_8"/>
-    <hyperlink ref="C107" r:id="rId229" tooltip="Dubnium"/>
-    <hyperlink ref="D107" r:id="rId230" tooltip="Dubna"/>
-    <hyperlink ref="G107" r:id="rId231" location="endnote_1"/>
-    <hyperlink ref="H107" r:id="rId232" location="endnote_11"/>
-    <hyperlink ref="M107" r:id="rId233" location="endnote_8"/>
-    <hyperlink ref="C108" r:id="rId234" tooltip="Seaborgium"/>
-    <hyperlink ref="D108" r:id="rId235" tooltip="Glenn T. Seaborg"/>
-    <hyperlink ref="G108" r:id="rId236" location="endnote_1"/>
-    <hyperlink ref="H108" r:id="rId237" location="endnote_11"/>
-    <hyperlink ref="M108" r:id="rId238" location="endnote_8"/>
-    <hyperlink ref="C109" r:id="rId239" tooltip="Bohrium"/>
-    <hyperlink ref="D109" r:id="rId240" tooltip="Niels Bohr"/>
-    <hyperlink ref="G109" r:id="rId241" location="endnote_1"/>
-    <hyperlink ref="H109" r:id="rId242" location="endnote_11"/>
-    <hyperlink ref="M109" r:id="rId243" location="endnote_8"/>
-    <hyperlink ref="C110" r:id="rId244" tooltip="Hassium"/>
-    <hyperlink ref="D110" r:id="rId245" tooltip="Hesse"/>
-    <hyperlink ref="G110" r:id="rId246" location="endnote_1"/>
-    <hyperlink ref="H110" r:id="rId247" location="endnote_11"/>
-    <hyperlink ref="M110" r:id="rId248" location="endnote_8"/>
-    <hyperlink ref="C111" r:id="rId249" tooltip="Meitnerium"/>
-    <hyperlink ref="D111" r:id="rId250" tooltip="Lise Meitner"/>
-    <hyperlink ref="G111" r:id="rId251" location="endnote_1"/>
-    <hyperlink ref="H111" r:id="rId252" location="endnote_11"/>
-    <hyperlink ref="M111" r:id="rId253" location="endnote_8"/>
-    <hyperlink ref="C112" r:id="rId254" tooltip="Darmstadtium"/>
-    <hyperlink ref="D112" r:id="rId255" tooltip="Darmstadt"/>
-    <hyperlink ref="G112" r:id="rId256" location="endnote_1"/>
-    <hyperlink ref="H112" r:id="rId257" location="endnote_11"/>
-    <hyperlink ref="M112" r:id="rId258" location="endnote_8"/>
-    <hyperlink ref="C113" r:id="rId259" tooltip="Roentgenium"/>
-    <hyperlink ref="D113" r:id="rId260" tooltip="Wilhelm Conrad Röntgen"/>
-    <hyperlink ref="G113" r:id="rId261" location="endnote_1"/>
-    <hyperlink ref="H113" r:id="rId262" location="endnote_11"/>
-    <hyperlink ref="M113" r:id="rId263" location="endnote_8"/>
-    <hyperlink ref="C114" r:id="rId264" tooltip="Copernicium"/>
-    <hyperlink ref="D114" r:id="rId265" tooltip="Nicolaus Copernicus"/>
-    <hyperlink ref="G114" r:id="rId266" location="endnote_1"/>
-    <hyperlink ref="H114" r:id="rId267" location="endnote_11"/>
-    <hyperlink ref="J114" r:id="rId268" location="endnote_12"/>
-    <hyperlink ref="M114" r:id="rId269" location="endnote_8"/>
-    <hyperlink ref="C115" r:id="rId270" tooltip="Ununtrium"/>
-    <hyperlink ref="G115" r:id="rId271" location="endnote_1"/>
-    <hyperlink ref="H115" r:id="rId272" location="endnote_11"/>
-    <hyperlink ref="I115" r:id="rId273" location="endnote_11"/>
-    <hyperlink ref="J115" r:id="rId274" location="endnote_11"/>
-    <hyperlink ref="M115" r:id="rId275" location="endnote_8"/>
-    <hyperlink ref="C116" r:id="rId276" tooltip="Flerovium"/>
-    <hyperlink ref="D116" r:id="rId277" tooltip="Georgy Flyorov"/>
-    <hyperlink ref="G116" r:id="rId278" location="endnote_1"/>
-    <hyperlink ref="H116" r:id="rId279" location="endnote_11"/>
-    <hyperlink ref="I116" r:id="rId280" location="endnote_11"/>
-    <hyperlink ref="J116" r:id="rId281" location="endnote_11"/>
-    <hyperlink ref="M116" r:id="rId282" location="endnote_8"/>
-    <hyperlink ref="C117" r:id="rId283" tooltip="Ununpentium"/>
-    <hyperlink ref="G117" r:id="rId284" location="endnote_1"/>
-    <hyperlink ref="H117" r:id="rId285" location="endnote_11"/>
-    <hyperlink ref="I117" r:id="rId286" location="endnote_11"/>
-    <hyperlink ref="J117" r:id="rId287" location="endnote_11"/>
-    <hyperlink ref="M117" r:id="rId288" location="endnote_8"/>
-    <hyperlink ref="C118" r:id="rId289" tooltip="Livermorium"/>
-    <hyperlink ref="G118" r:id="rId290" location="endnote_1"/>
-    <hyperlink ref="H118" r:id="rId291" location="endnote_11"/>
-    <hyperlink ref="I118" r:id="rId292" location="endnote_11"/>
-    <hyperlink ref="J118" r:id="rId293" location="endnote_11"/>
-    <hyperlink ref="M118" r:id="rId294" location="endnote_8"/>
-    <hyperlink ref="C119" r:id="rId295" tooltip="Ununseptium"/>
-    <hyperlink ref="G119" r:id="rId296" location="endnote_1"/>
-    <hyperlink ref="H119" r:id="rId297" location="endnote_11"/>
-    <hyperlink ref="I119" r:id="rId298" location="endnote_11"/>
-    <hyperlink ref="J119" r:id="rId299" location="endnote_11"/>
-    <hyperlink ref="M119" r:id="rId300" location="endnote_8"/>
-    <hyperlink ref="C120" r:id="rId301" tooltip="Ununoctium"/>
-    <hyperlink ref="G120" r:id="rId302" location="endnote_1"/>
-    <hyperlink ref="I120" r:id="rId303" location="endnote_11"/>
-    <hyperlink ref="J120" r:id="rId304" location="endnote_11"/>
-    <hyperlink ref="M120" r:id="rId305" location="endnote_8"/>
+    <hyperlink ref="C15" r:id="rId31" tooltip="Aluminium"/>
+    <hyperlink ref="C16" r:id="rId32" tooltip="Silicon"/>
+    <hyperlink ref="C17" r:id="rId33" tooltip="Phosphorus"/>
+    <hyperlink ref="C18" r:id="rId34" tooltip="Sulfur"/>
+    <hyperlink ref="C19" r:id="rId35" tooltip="Chlorine"/>
+    <hyperlink ref="C20" r:id="rId36" tooltip="Argon"/>
+    <hyperlink ref="C21" r:id="rId37" tooltip="Potassium"/>
+    <hyperlink ref="D21" r:id="rId38" location="cite_note-innvista-2"/>
+    <hyperlink ref="C22" r:id="rId39" tooltip="Calcium"/>
+    <hyperlink ref="G22" r:id="rId40" location="endnote_2"/>
+    <hyperlink ref="C23" r:id="rId41" tooltip="Scandium"/>
+    <hyperlink ref="D23" r:id="rId42" tooltip="Scandinavia"/>
+    <hyperlink ref="C24" r:id="rId43" tooltip="Titanium"/>
+    <hyperlink ref="D24" r:id="rId44" tooltip="Titan (mythology)"/>
+    <hyperlink ref="C25" r:id="rId45" tooltip="Vanadium"/>
+    <hyperlink ref="C26" r:id="rId46" tooltip="Chromium"/>
+    <hyperlink ref="C27" r:id="rId47" tooltip="Manganese"/>
+    <hyperlink ref="C28" r:id="rId48" tooltip="Iron"/>
+    <hyperlink ref="D28" r:id="rId49" tooltip="Anglo-Saxon"/>
+    <hyperlink ref="C29" r:id="rId50" tooltip="Cobalt"/>
+    <hyperlink ref="D29" r:id="rId51" tooltip="German language"/>
+    <hyperlink ref="C30" r:id="rId52" tooltip="Nickel"/>
+    <hyperlink ref="C31" r:id="rId53" tooltip="Copper"/>
+    <hyperlink ref="D31" r:id="rId54" tooltip="Cyprus"/>
+    <hyperlink ref="G31" r:id="rId55" location="endnote_4"/>
+    <hyperlink ref="C32" r:id="rId56" tooltip="Zinc"/>
+    <hyperlink ref="D32" r:id="rId57" tooltip="Persian language"/>
+    <hyperlink ref="C33" r:id="rId58" tooltip="Gallium"/>
+    <hyperlink ref="D33" r:id="rId59" tooltip="France"/>
+    <hyperlink ref="C34" r:id="rId60" tooltip="Germanium"/>
+    <hyperlink ref="D34" r:id="rId61" tooltip="Germany"/>
+    <hyperlink ref="C35" r:id="rId62" tooltip="Arsenic"/>
+    <hyperlink ref="D35" r:id="rId63" tooltip="Orpiment"/>
+    <hyperlink ref="I35" r:id="rId64" location="endnote_7"/>
+    <hyperlink ref="C36" r:id="rId65" tooltip="Selenium"/>
+    <hyperlink ref="D36" r:id="rId66" tooltip="Moon"/>
+    <hyperlink ref="G36" r:id="rId67" location="endnote_4"/>
+    <hyperlink ref="C37" r:id="rId68" tooltip="Bromine"/>
+    <hyperlink ref="G37" r:id="rId69" location="endnote_9" display="https://en.wikipedia.org/wiki/List_of_elements - endnote_9"/>
+    <hyperlink ref="C38" r:id="rId70" tooltip="Krypton"/>
+    <hyperlink ref="C39" r:id="rId71" tooltip="Rubidium"/>
+    <hyperlink ref="G39" r:id="rId72" location="endnote_2"/>
+    <hyperlink ref="C40" r:id="rId73" tooltip="Strontium"/>
+    <hyperlink ref="C41" r:id="rId74" tooltip="Yttrium"/>
+    <hyperlink ref="C42" r:id="rId75" tooltip="Zirconium"/>
+    <hyperlink ref="G42" r:id="rId76" location="endnote_2"/>
+    <hyperlink ref="C43" r:id="rId77" tooltip="Niobium"/>
+    <hyperlink ref="C44" r:id="rId78" tooltip="Molybdenum"/>
+    <hyperlink ref="G44" r:id="rId79" location="endnote_2"/>
+    <hyperlink ref="C45" r:id="rId80" tooltip="Technetium"/>
+    <hyperlink ref="G45" r:id="rId81" location="endnote_1"/>
+    <hyperlink ref="C46" r:id="rId82" tooltip="Ruthenium"/>
+    <hyperlink ref="D46" r:id="rId83" tooltip="Russia"/>
+    <hyperlink ref="G46" r:id="rId84" location="endnote_2"/>
+    <hyperlink ref="C47" r:id="rId85" tooltip="Rhodium"/>
+    <hyperlink ref="C48" r:id="rId86" tooltip="Palladium"/>
+    <hyperlink ref="D48" r:id="rId87" tooltip="2 Pallas"/>
+    <hyperlink ref="G48" r:id="rId88" location="endnote_2"/>
+    <hyperlink ref="C49" r:id="rId89" tooltip="Silver"/>
+    <hyperlink ref="G49" r:id="rId90" location="endnote_2"/>
+    <hyperlink ref="C50" r:id="rId91" tooltip="Cadmium"/>
+    <hyperlink ref="G50" r:id="rId92" location="endnote_2"/>
+    <hyperlink ref="C51" r:id="rId93" tooltip="Indium"/>
+    <hyperlink ref="C52" r:id="rId94" tooltip="Tin"/>
+    <hyperlink ref="G52" r:id="rId95" location="endnote_2"/>
+    <hyperlink ref="C53" r:id="rId96" tooltip="Antimony"/>
+    <hyperlink ref="G53" r:id="rId97" location="endnote_2"/>
+    <hyperlink ref="C54" r:id="rId98" tooltip="Tellurium"/>
+    <hyperlink ref="G54" r:id="rId99" location="endnote_2"/>
+    <hyperlink ref="C55" r:id="rId100" tooltip="Iodine"/>
+    <hyperlink ref="C56" r:id="rId101" tooltip="Xenon"/>
+    <hyperlink ref="C57" r:id="rId102" tooltip="Caesium"/>
+    <hyperlink ref="C58" r:id="rId103" tooltip="Barium"/>
+    <hyperlink ref="C59" r:id="rId104" tooltip="Lanthanum"/>
+    <hyperlink ref="G59" r:id="rId105" location="endnote_2"/>
+    <hyperlink ref="C60" r:id="rId106" tooltip="Cerium"/>
+    <hyperlink ref="G60" r:id="rId107" location="endnote_2"/>
+    <hyperlink ref="C61" r:id="rId108" tooltip="Praseodymium"/>
+    <hyperlink ref="C62" r:id="rId109" tooltip="Neodymium"/>
+    <hyperlink ref="G62" r:id="rId110" location="endnote_2"/>
+    <hyperlink ref="C63" r:id="rId111" tooltip="Promethium"/>
+    <hyperlink ref="D63" r:id="rId112" tooltip="Prometheus"/>
+    <hyperlink ref="G63" r:id="rId113" location="endnote_1"/>
+    <hyperlink ref="C64" r:id="rId114" tooltip="Samarium"/>
+    <hyperlink ref="D64" r:id="rId115" tooltip="Samarskite"/>
+    <hyperlink ref="G64" r:id="rId116" location="endnote_2"/>
+    <hyperlink ref="C65" r:id="rId117" tooltip="Europium"/>
+    <hyperlink ref="D65" r:id="rId118" tooltip="Europe"/>
+    <hyperlink ref="G65" r:id="rId119" location="endnote_2"/>
+    <hyperlink ref="C66" r:id="rId120" tooltip="Gadolinium"/>
+    <hyperlink ref="D66" r:id="rId121" tooltip="Johan Gadolin"/>
+    <hyperlink ref="G66" r:id="rId122" location="endnote_2"/>
+    <hyperlink ref="C67" r:id="rId123" tooltip="Terbium"/>
+    <hyperlink ref="C68" r:id="rId124" tooltip="Dysprosium"/>
+    <hyperlink ref="G68" r:id="rId125" location="endnote_2"/>
+    <hyperlink ref="C69" r:id="rId126" tooltip="Holmium"/>
+    <hyperlink ref="D69" r:id="rId127" tooltip="Stockholm"/>
+    <hyperlink ref="C70" r:id="rId128" tooltip="Erbium"/>
+    <hyperlink ref="G70" r:id="rId129" location="endnote_2"/>
+    <hyperlink ref="C71" r:id="rId130" tooltip="Thulium"/>
+    <hyperlink ref="D71" r:id="rId131" tooltip="Thule"/>
+    <hyperlink ref="C72" r:id="rId132" tooltip="Ytterbium"/>
+    <hyperlink ref="G72" r:id="rId133" location="endnote_2"/>
+    <hyperlink ref="C73" r:id="rId134" tooltip="Lutetium"/>
+    <hyperlink ref="D73" r:id="rId135" tooltip="Paris"/>
+    <hyperlink ref="G73" r:id="rId136" location="endnote_2"/>
+    <hyperlink ref="C74" r:id="rId137" tooltip="Hafnium"/>
+    <hyperlink ref="D74" r:id="rId138" tooltip="Copenhagen"/>
+    <hyperlink ref="C75" r:id="rId139" tooltip="Tantalum"/>
+    <hyperlink ref="D75" r:id="rId140" tooltip="Tantalus"/>
+    <hyperlink ref="C76" r:id="rId141" tooltip="Tungsten"/>
+    <hyperlink ref="D76" r:id="rId142" location="cite_note-innvista-2"/>
+    <hyperlink ref="C77" r:id="rId143" tooltip="Rhenium"/>
+    <hyperlink ref="C78" r:id="rId144" tooltip="Osmium"/>
+    <hyperlink ref="G78" r:id="rId145" location="endnote_2"/>
+    <hyperlink ref="C79" r:id="rId146" tooltip="Iridium"/>
+    <hyperlink ref="D79" r:id="rId147" tooltip="Iris (mythology)"/>
+    <hyperlink ref="C80" r:id="rId148" tooltip="Platinum"/>
+    <hyperlink ref="D80" r:id="rId149" tooltip="Spanish language"/>
+    <hyperlink ref="C81" r:id="rId150" tooltip="Gold"/>
+    <hyperlink ref="D81" r:id="rId151" location="cite_note-innvista-2"/>
+    <hyperlink ref="C82" r:id="rId152" tooltip="Mercury (element)"/>
+    <hyperlink ref="C83" r:id="rId153" tooltip="Thallium"/>
+    <hyperlink ref="G83" r:id="rId154" location="endnote_9" display="https://en.wikipedia.org/wiki/List_of_elements - endnote_9"/>
+    <hyperlink ref="C84" r:id="rId155" tooltip="Lead"/>
+    <hyperlink ref="D84" r:id="rId156" location="cite_note-innvista-2"/>
+    <hyperlink ref="C85" r:id="rId157" tooltip="Bismuth"/>
+    <hyperlink ref="G85" r:id="rId158" location="endnote_1"/>
+    <hyperlink ref="C86" r:id="rId159" tooltip="Polonium"/>
+    <hyperlink ref="G86" r:id="rId160" location="endnote_1"/>
+    <hyperlink ref="C87" r:id="rId161" tooltip="Astatine"/>
+    <hyperlink ref="G87" r:id="rId162" location="endnote_1"/>
+    <hyperlink ref="C88" r:id="rId163" tooltip="Radon"/>
+    <hyperlink ref="G88" r:id="rId164" location="endnote_1"/>
+    <hyperlink ref="C89" r:id="rId165" tooltip="Francium"/>
+    <hyperlink ref="G89" r:id="rId166" location="endnote_1"/>
+    <hyperlink ref="C90" r:id="rId167" tooltip="Radium"/>
+    <hyperlink ref="G90" r:id="rId168" location="endnote_1"/>
+    <hyperlink ref="C91" r:id="rId169" tooltip="Actinium"/>
+    <hyperlink ref="G91" r:id="rId170" location="endnote_1"/>
+    <hyperlink ref="C92" r:id="rId171" tooltip="Thorium"/>
+    <hyperlink ref="D92" r:id="rId172" tooltip="Thor"/>
+    <hyperlink ref="C93" r:id="rId173" tooltip="Protactinium"/>
+    <hyperlink ref="G93" r:id="rId174" location="endnote_1"/>
+    <hyperlink ref="C94" r:id="rId175" tooltip="Uranium"/>
+    <hyperlink ref="D94" r:id="rId176" tooltip="Uranus"/>
+    <hyperlink ref="G94" r:id="rId177" location="endnote_1"/>
+    <hyperlink ref="C95" r:id="rId178" tooltip="Neptunium"/>
+    <hyperlink ref="D95" r:id="rId179" tooltip="Neptune"/>
+    <hyperlink ref="G95" r:id="rId180" location="endnote_1"/>
+    <hyperlink ref="C96" r:id="rId181" tooltip="Plutonium"/>
+    <hyperlink ref="D96" r:id="rId182" tooltip="Pluto"/>
+    <hyperlink ref="G96" r:id="rId183" location="endnote_1"/>
+    <hyperlink ref="C97" r:id="rId184" tooltip="Americium"/>
+    <hyperlink ref="D97" r:id="rId185" tooltip="Americas"/>
+    <hyperlink ref="G97" r:id="rId186" location="endnote_1"/>
+    <hyperlink ref="C98" r:id="rId187" tooltip="Curium"/>
+    <hyperlink ref="G98" r:id="rId188" location="endnote_1"/>
+    <hyperlink ref="C99" r:id="rId189" tooltip="Berkelium"/>
+    <hyperlink ref="D99" r:id="rId190" tooltip="Berkeley, California"/>
+    <hyperlink ref="G99" r:id="rId191" location="endnote_1"/>
+    <hyperlink ref="C100" r:id="rId192" tooltip="Californium"/>
+    <hyperlink ref="D100" r:id="rId193" tooltip="State of California"/>
+    <hyperlink ref="G100" r:id="rId194" location="endnote_1"/>
+    <hyperlink ref="J100" r:id="rId195" location="endnote_11"/>
+    <hyperlink ref="C101" r:id="rId196" tooltip="Einsteinium"/>
+    <hyperlink ref="D101" r:id="rId197" tooltip="Albert Einstein"/>
+    <hyperlink ref="G101" r:id="rId198" location="endnote_1"/>
+    <hyperlink ref="J101" r:id="rId199" location="endnote_11"/>
+    <hyperlink ref="M101" r:id="rId200" location="endnote_8"/>
+    <hyperlink ref="C102" r:id="rId201" tooltip="Fermium"/>
+    <hyperlink ref="D102" r:id="rId202" tooltip="Enrico Fermi"/>
+    <hyperlink ref="G102" r:id="rId203" location="endnote_1"/>
+    <hyperlink ref="I102" r:id="rId204" location="endnote_11"/>
+    <hyperlink ref="M102" r:id="rId205" location="endnote_8"/>
+    <hyperlink ref="C103" r:id="rId206" tooltip="Mendelevium"/>
+    <hyperlink ref="D103" r:id="rId207" tooltip="Dmitri Mendeleyev"/>
+    <hyperlink ref="G103" r:id="rId208" location="endnote_1"/>
+    <hyperlink ref="I103" r:id="rId209" location="endnote_11"/>
+    <hyperlink ref="M103" r:id="rId210" location="endnote_8"/>
+    <hyperlink ref="C104" r:id="rId211" tooltip="Nobelium"/>
+    <hyperlink ref="D104" r:id="rId212" tooltip="Alfred Nobel"/>
+    <hyperlink ref="G104" r:id="rId213" location="endnote_1"/>
+    <hyperlink ref="I104" r:id="rId214" location="endnote_11"/>
+    <hyperlink ref="M104" r:id="rId215" location="endnote_8"/>
+    <hyperlink ref="C105" r:id="rId216" tooltip="Lawrencium"/>
+    <hyperlink ref="D105" r:id="rId217" tooltip="Ernest O. Lawrence"/>
+    <hyperlink ref="G105" r:id="rId218" location="endnote_1"/>
+    <hyperlink ref="I105" r:id="rId219" location="endnote_11"/>
+    <hyperlink ref="M105" r:id="rId220" location="endnote_8"/>
+    <hyperlink ref="C106" r:id="rId221" tooltip="Rutherfordium"/>
+    <hyperlink ref="D106" r:id="rId222" tooltip="Ernest Rutherford"/>
+    <hyperlink ref="G106" r:id="rId223" location="endnote_1"/>
+    <hyperlink ref="H106" r:id="rId224" location="endnote_11"/>
+    <hyperlink ref="I106" r:id="rId225" location="endnote_11"/>
+    <hyperlink ref="J106" r:id="rId226" location="endnote_11"/>
+    <hyperlink ref="M106" r:id="rId227" location="endnote_8"/>
+    <hyperlink ref="C107" r:id="rId228" tooltip="Dubnium"/>
+    <hyperlink ref="D107" r:id="rId229" tooltip="Dubna"/>
+    <hyperlink ref="G107" r:id="rId230" location="endnote_1"/>
+    <hyperlink ref="H107" r:id="rId231" location="endnote_11"/>
+    <hyperlink ref="M107" r:id="rId232" location="endnote_8"/>
+    <hyperlink ref="C108" r:id="rId233" tooltip="Seaborgium"/>
+    <hyperlink ref="D108" r:id="rId234" tooltip="Glenn T. Seaborg"/>
+    <hyperlink ref="G108" r:id="rId235" location="endnote_1"/>
+    <hyperlink ref="H108" r:id="rId236" location="endnote_11"/>
+    <hyperlink ref="M108" r:id="rId237" location="endnote_8"/>
+    <hyperlink ref="C109" r:id="rId238" tooltip="Bohrium"/>
+    <hyperlink ref="D109" r:id="rId239" tooltip="Niels Bohr"/>
+    <hyperlink ref="G109" r:id="rId240" location="endnote_1"/>
+    <hyperlink ref="H109" r:id="rId241" location="endnote_11"/>
+    <hyperlink ref="M109" r:id="rId242" location="endnote_8"/>
+    <hyperlink ref="C110" r:id="rId243" tooltip="Hassium"/>
+    <hyperlink ref="D110" r:id="rId244" tooltip="Hesse"/>
+    <hyperlink ref="G110" r:id="rId245" location="endnote_1"/>
+    <hyperlink ref="H110" r:id="rId246" location="endnote_11"/>
+    <hyperlink ref="M110" r:id="rId247" location="endnote_8"/>
+    <hyperlink ref="C111" r:id="rId248" tooltip="Meitnerium"/>
+    <hyperlink ref="D111" r:id="rId249" tooltip="Lise Meitner"/>
+    <hyperlink ref="G111" r:id="rId250" location="endnote_1"/>
+    <hyperlink ref="H111" r:id="rId251" location="endnote_11"/>
+    <hyperlink ref="M111" r:id="rId252" location="endnote_8"/>
+    <hyperlink ref="C112" r:id="rId253" tooltip="Darmstadtium"/>
+    <hyperlink ref="D112" r:id="rId254" tooltip="Darmstadt"/>
+    <hyperlink ref="G112" r:id="rId255" location="endnote_1"/>
+    <hyperlink ref="H112" r:id="rId256" location="endnote_11"/>
+    <hyperlink ref="M112" r:id="rId257" location="endnote_8"/>
+    <hyperlink ref="C113" r:id="rId258" tooltip="Roentgenium"/>
+    <hyperlink ref="D113" r:id="rId259" tooltip="Wilhelm Conrad Röntgen"/>
+    <hyperlink ref="G113" r:id="rId260" location="endnote_1"/>
+    <hyperlink ref="H113" r:id="rId261" location="endnote_11"/>
+    <hyperlink ref="M113" r:id="rId262" location="endnote_8"/>
+    <hyperlink ref="C114" r:id="rId263" tooltip="Copernicium"/>
+    <hyperlink ref="D114" r:id="rId264" tooltip="Nicolaus Copernicus"/>
+    <hyperlink ref="G114" r:id="rId265" location="endnote_1"/>
+    <hyperlink ref="H114" r:id="rId266" location="endnote_11"/>
+    <hyperlink ref="J114" r:id="rId267" location="endnote_12"/>
+    <hyperlink ref="M114" r:id="rId268" location="endnote_8"/>
+    <hyperlink ref="C115" r:id="rId269" tooltip="Ununtrium"/>
+    <hyperlink ref="G115" r:id="rId270" location="endnote_1"/>
+    <hyperlink ref="H115" r:id="rId271" location="endnote_11"/>
+    <hyperlink ref="I115" r:id="rId272" location="endnote_11"/>
+    <hyperlink ref="J115" r:id="rId273" location="endnote_11"/>
+    <hyperlink ref="M115" r:id="rId274" location="endnote_8"/>
+    <hyperlink ref="C116" r:id="rId275" tooltip="Flerovium"/>
+    <hyperlink ref="D116" r:id="rId276" tooltip="Georgy Flyorov"/>
+    <hyperlink ref="G116" r:id="rId277" location="endnote_1"/>
+    <hyperlink ref="H116" r:id="rId278" location="endnote_11"/>
+    <hyperlink ref="I116" r:id="rId279" location="endnote_11"/>
+    <hyperlink ref="J116" r:id="rId280" location="endnote_11"/>
+    <hyperlink ref="M116" r:id="rId281" location="endnote_8"/>
+    <hyperlink ref="C117" r:id="rId282" tooltip="Ununpentium"/>
+    <hyperlink ref="G117" r:id="rId283" location="endnote_1"/>
+    <hyperlink ref="H117" r:id="rId284" location="endnote_11"/>
+    <hyperlink ref="I117" r:id="rId285" location="endnote_11"/>
+    <hyperlink ref="J117" r:id="rId286" location="endnote_11"/>
+    <hyperlink ref="M117" r:id="rId287" location="endnote_8"/>
+    <hyperlink ref="C118" r:id="rId288" tooltip="Livermorium"/>
+    <hyperlink ref="G118" r:id="rId289" location="endnote_1"/>
+    <hyperlink ref="H118" r:id="rId290" location="endnote_11"/>
+    <hyperlink ref="I118" r:id="rId291" location="endnote_11"/>
+    <hyperlink ref="J118" r:id="rId292" location="endnote_11"/>
+    <hyperlink ref="M118" r:id="rId293" location="endnote_8"/>
+    <hyperlink ref="C119" r:id="rId294" tooltip="Ununseptium"/>
+    <hyperlink ref="G119" r:id="rId295" location="endnote_1"/>
+    <hyperlink ref="H119" r:id="rId296" location="endnote_11"/>
+    <hyperlink ref="I119" r:id="rId297" location="endnote_11"/>
+    <hyperlink ref="J119" r:id="rId298" location="endnote_11"/>
+    <hyperlink ref="M119" r:id="rId299" location="endnote_8"/>
+    <hyperlink ref="C120" r:id="rId300" tooltip="Ununoctium"/>
+    <hyperlink ref="G120" r:id="rId301" location="endnote_1"/>
+    <hyperlink ref="I120" r:id="rId302" location="endnote_11"/>
+    <hyperlink ref="J120" r:id="rId303" location="endnote_11"/>
+    <hyperlink ref="M120" r:id="rId304" location="endnote_8"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Before importing elements.csv into elements.sqlite
</commit_message>
<xml_diff>
--- a/Elements.xlsx
+++ b/Elements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="409">
   <si>
     <t>abundance_mg_per_kg</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -43,6 +43,10 @@
   </si>
   <si>
     <t>specific_heat_capacity_J_per_gK</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>–</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -2496,11 +2500,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:V119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2515,64 +2519,64 @@
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" ht="65">
       <c r="A1" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="U1" s="12" t="s">
         <v>0</v>
@@ -2586,13 +2590,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -2658,13 +2662,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1">
         <v>18</v>
@@ -2711,9 +2715,7 @@
         <f>IF(ISERR(FIND(")11",J3))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S3" s="1"/>
       <c r="T3" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -2730,13 +2732,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -2802,13 +2804,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -2874,13 +2876,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1">
         <v>13</v>
@@ -2946,13 +2948,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1">
         <v>14</v>
@@ -3018,13 +3020,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1">
         <v>15</v>
@@ -3090,13 +3092,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1">
         <v>16</v>
@@ -3162,13 +3164,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1">
         <v>17</v>
@@ -3234,13 +3236,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1">
         <v>18</v>
@@ -3287,9 +3289,7 @@
         <f>IF(ISERR(FIND(")11",J11))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S11" s="1"/>
       <c r="T11" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -3306,13 +3306,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -3378,13 +3378,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
@@ -3450,13 +3450,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E14" s="1">
         <v>13</v>
@@ -3522,13 +3522,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1">
         <v>14</v>
@@ -3594,13 +3594,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E16" s="1">
         <v>15</v>
@@ -3666,13 +3666,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1">
         <v>16</v>
@@ -3738,13 +3738,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E18" s="1">
         <v>17</v>
@@ -3810,13 +3810,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E19" s="1">
         <v>18</v>
@@ -3863,9 +3863,7 @@
         <f>IF(ISERR(FIND(")11",J19))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S19" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S19" s="1"/>
       <c r="T19" s="1">
         <v>3.5</v>
       </c>
@@ -3882,13 +3880,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -3954,13 +3952,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
@@ -4026,13 +4024,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E22" s="1">
         <v>3</v>
@@ -4098,13 +4096,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D23" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E23" s="1">
         <v>4</v>
@@ -4170,13 +4168,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E24" s="1">
         <v>5</v>
@@ -4242,13 +4240,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E25" s="1">
         <v>6</v>
@@ -4314,13 +4312,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E26" s="1">
         <v>7</v>
@@ -4386,13 +4384,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E27" s="1">
         <v>8</v>
@@ -4458,13 +4456,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D28" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E28" s="1">
         <v>9</v>
@@ -4530,13 +4528,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E29" s="1">
         <v>10</v>
@@ -4602,13 +4600,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E30" s="1">
         <v>11</v>
@@ -4674,13 +4672,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E31" s="1">
         <v>12</v>
@@ -4746,13 +4744,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E32" s="1">
         <v>13</v>
@@ -4818,13 +4816,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D33" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E33" s="1">
         <v>14</v>
@@ -4890,13 +4888,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D34" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E34" s="1">
         <v>15</v>
@@ -4962,13 +4960,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D35" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E35" s="1">
         <v>16</v>
@@ -5034,13 +5032,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E36" s="1">
         <v>17</v>
@@ -5106,13 +5104,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E37" s="1">
         <v>18</v>
@@ -5163,7 +5161,7 @@
         <v>3</v>
       </c>
       <c r="T37" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U37">
         <v>1E-3</v>
@@ -5178,13 +5176,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -5250,13 +5248,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E39" s="1">
         <v>2</v>
@@ -5322,13 +5320,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E40" s="1">
         <v>3</v>
@@ -5394,13 +5392,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E41" s="1">
         <v>4</v>
@@ -5466,13 +5464,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E42" s="1">
         <v>5</v>
@@ -5538,13 +5536,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E43" s="1">
         <v>6</v>
@@ -5610,13 +5608,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E44" s="1">
         <v>7</v>
@@ -5640,7 +5638,7 @@
         <v>1</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="M44" s="1">
         <v>11.5</v>
@@ -5667,7 +5665,7 @@
         <v>1.9</v>
       </c>
       <c r="T44" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U44">
         <v>1E-3</v>
@@ -5682,13 +5680,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D45" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E45" s="1">
         <v>8</v>
@@ -5754,13 +5752,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E46" s="1">
         <v>9</v>
@@ -5826,13 +5824,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D47" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E47" s="1">
         <v>10</v>
@@ -5898,13 +5896,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E48" s="1">
         <v>11</v>
@@ -5970,13 +5968,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E49" s="1">
         <v>12</v>
@@ -6042,13 +6040,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E50" s="1">
         <v>13</v>
@@ -6114,13 +6112,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E51" s="1">
         <v>14</v>
@@ -6186,13 +6184,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E52" s="1">
         <v>15</v>
@@ -6258,13 +6256,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E53" s="1">
         <v>16</v>
@@ -6330,13 +6328,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E54" s="1">
         <v>17</v>
@@ -6402,13 +6400,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E55" s="1">
         <v>18</v>
@@ -6459,7 +6457,7 @@
         <v>2.6</v>
       </c>
       <c r="T55" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U55">
         <v>1E-3</v>
@@ -6474,13 +6472,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E56" s="1">
         <v>1</v>
@@ -6546,13 +6544,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E57" s="1">
         <v>2</v>
@@ -6618,13 +6616,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1">
@@ -6688,13 +6686,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1">
@@ -6758,13 +6756,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1">
@@ -6828,13 +6826,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1">
@@ -6898,13 +6896,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D62" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1">
@@ -6925,9 +6923,7 @@
       <c r="K62" s="1">
         <v>1</v>
       </c>
-      <c r="L62" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L62" s="1"/>
       <c r="M62" s="1">
         <v>7.26</v>
       </c>
@@ -6953,7 +6949,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="T62" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="U62">
         <v>1E-3</v>
@@ -6968,13 +6964,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D63" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1">
@@ -7038,13 +7034,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D64" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1">
@@ -7108,13 +7104,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D65" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1">
@@ -7178,13 +7174,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1">
@@ -7248,13 +7244,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1">
@@ -7318,13 +7314,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D68" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1">
@@ -7388,13 +7384,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1">
@@ -7458,13 +7454,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D70" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1">
@@ -7528,13 +7524,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1">
@@ -7598,13 +7594,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D72" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E72" s="1">
         <v>3</v>
@@ -7670,13 +7666,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D73" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E73" s="1">
         <v>4</v>
@@ -7742,13 +7738,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D74" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E74" s="1">
         <v>5</v>
@@ -7814,13 +7810,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D75" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E75" s="1">
         <v>6</v>
@@ -7886,13 +7882,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E76" s="1">
         <v>7</v>
@@ -7943,10 +7939,10 @@
         <v>1.9</v>
       </c>
       <c r="T76" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U76" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U76">
+        <v>1E-3</v>
       </c>
       <c r="V76">
         <f t="shared" si="1"/>
@@ -7958,13 +7954,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E77" s="1">
         <v>8</v>
@@ -8030,13 +8026,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D78" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E78" s="1">
         <v>9</v>
@@ -8102,13 +8098,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D79" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E79" s="1">
         <v>10</v>
@@ -8174,13 +8170,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D80" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E80" s="1">
         <v>11</v>
@@ -8246,13 +8242,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E81" s="1">
         <v>12</v>
@@ -8318,13 +8314,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E82" s="1">
         <v>13</v>
@@ -8390,13 +8386,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D83" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E83" s="1">
         <v>14</v>
@@ -8462,13 +8458,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E84" s="1">
         <v>15</v>
@@ -8534,13 +8530,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E85" s="1">
         <v>16</v>
@@ -8563,9 +8559,7 @@
       <c r="K85" s="1">
         <v>1</v>
       </c>
-      <c r="L85" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L85" s="1"/>
       <c r="M85" s="1">
         <v>9.32</v>
       </c>
@@ -8591,10 +8585,10 @@
         <v>2</v>
       </c>
       <c r="T85" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U85" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U85">
+        <v>1E-3</v>
       </c>
       <c r="V85">
         <f t="shared" si="1"/>
@@ -8606,13 +8600,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E86" s="1">
         <v>17</v>
@@ -8635,9 +8629,7 @@
       <c r="K86" s="1">
         <v>1</v>
       </c>
-      <c r="L86" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L86" s="1"/>
       <c r="M86" s="1">
         <v>7</v>
       </c>
@@ -8663,10 +8655,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="T86" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U86" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U86">
+        <v>1E-3</v>
       </c>
       <c r="V86">
         <f t="shared" si="1"/>
@@ -8678,13 +8670,13 @@
         <v>86</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E87" s="1">
         <v>18</v>
@@ -8735,10 +8727,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="T87" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U87" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U87">
+        <v>1E-3</v>
       </c>
       <c r="V87">
         <f t="shared" si="1"/>
@@ -8750,13 +8742,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E88" s="1">
         <v>1</v>
@@ -8779,9 +8771,7 @@
       <c r="K88" s="1">
         <v>1</v>
       </c>
-      <c r="L88" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L88" s="1"/>
       <c r="M88" s="1">
         <v>1.87</v>
       </c>
@@ -8807,10 +8797,10 @@
         <v>0.7</v>
       </c>
       <c r="T88" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U88" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U88">
+        <v>1E-3</v>
       </c>
       <c r="V88">
         <f t="shared" si="1"/>
@@ -8822,13 +8812,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E89" s="1">
         <v>2</v>
@@ -8879,10 +8869,10 @@
         <v>0.9</v>
       </c>
       <c r="T89" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U89" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U89">
+        <v>1E-3</v>
       </c>
       <c r="V89">
         <f t="shared" si="1"/>
@@ -8894,13 +8884,13 @@
         <v>89</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1">
@@ -8949,10 +8939,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="T90" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U90" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U90">
+        <v>1E-3</v>
       </c>
       <c r="V90">
         <f t="shared" si="1"/>
@@ -8964,13 +8954,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D91" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1">
@@ -9034,13 +9024,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1">
@@ -9061,9 +9051,7 @@
       <c r="K92" s="1">
         <v>0</v>
       </c>
-      <c r="L92" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L92" s="1"/>
       <c r="M92" s="1">
         <v>15.37</v>
       </c>
@@ -9089,10 +9077,10 @@
         <v>1.5</v>
       </c>
       <c r="T92" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U92" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U92">
+        <v>1E-3</v>
       </c>
       <c r="V92">
         <f t="shared" si="1"/>
@@ -9104,13 +9092,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D93" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1">
@@ -9174,13 +9162,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D94" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1">
@@ -9201,9 +9189,7 @@
       <c r="K94" s="1">
         <v>1</v>
       </c>
-      <c r="L94" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L94" s="1"/>
       <c r="M94" s="1">
         <v>20.45</v>
       </c>
@@ -9229,10 +9215,10 @@
         <v>1.36</v>
       </c>
       <c r="T94" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U94" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U94">
+        <v>1E-3</v>
       </c>
       <c r="V94">
         <f t="shared" si="1"/>
@@ -9244,13 +9230,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D95" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1">
@@ -9271,9 +9257,7 @@
       <c r="K95" s="1">
         <v>1</v>
       </c>
-      <c r="L95" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L95" s="1"/>
       <c r="M95" s="1">
         <v>19.84</v>
       </c>
@@ -9299,10 +9283,10 @@
         <v>1.28</v>
       </c>
       <c r="T95" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U95" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U95">
+        <v>1E-3</v>
       </c>
       <c r="V95">
         <f t="shared" si="1"/>
@@ -9314,13 +9298,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D96" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1">
@@ -9341,9 +9325,7 @@
       <c r="K96" s="1">
         <v>1</v>
       </c>
-      <c r="L96" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L96" s="1"/>
       <c r="M96" s="1">
         <v>13.69</v>
       </c>
@@ -9369,10 +9351,10 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="T96" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U96" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U96">
+        <v>1E-3</v>
       </c>
       <c r="V96">
         <f t="shared" si="1"/>
@@ -9384,13 +9366,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1">
@@ -9411,9 +9393,7 @@
       <c r="K97" s="1">
         <v>1</v>
       </c>
-      <c r="L97" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L97" s="1"/>
       <c r="M97" s="1">
         <v>13.51</v>
       </c>
@@ -9439,10 +9419,10 @@
         <v>1.28</v>
       </c>
       <c r="T97" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U97" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U97">
+        <v>1E-3</v>
       </c>
       <c r="V97">
         <f t="shared" si="1"/>
@@ -9454,13 +9434,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D98" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1">
@@ -9481,9 +9461,7 @@
       <c r="K98" s="1">
         <v>1</v>
       </c>
-      <c r="L98" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L98" s="1"/>
       <c r="M98" s="1">
         <v>14.79</v>
       </c>
@@ -9509,10 +9487,10 @@
         <v>1.3</v>
       </c>
       <c r="T98" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U98" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U98">
+        <v>1E-3</v>
       </c>
       <c r="V98">
         <f t="shared" si="1"/>
@@ -9524,13 +9502,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D99" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1">
@@ -9546,14 +9524,12 @@
         <v>1173</v>
       </c>
       <c r="J99" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="K99" s="1">
         <v>1</v>
       </c>
-      <c r="L99" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L99" s="1"/>
       <c r="M99" s="1">
         <v>15.1</v>
       </c>
@@ -9579,10 +9555,10 @@
         <v>1.3</v>
       </c>
       <c r="T99" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U99" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="U99">
+        <v>1E-3</v>
       </c>
       <c r="V99">
         <f t="shared" si="1"/>
@@ -9594,13 +9570,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D100" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1">
@@ -9616,14 +9592,12 @@
         <v>1133</v>
       </c>
       <c r="J100" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="K100">
         <v>1</v>
       </c>
-      <c r="L100" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L100" s="1"/>
       <c r="M100" s="1">
         <v>8.84</v>
       </c>
@@ -9649,7 +9623,7 @@
         <v>1.3</v>
       </c>
       <c r="T100" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U100">
         <v>0</v>
@@ -9664,13 +9638,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D101" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1">
@@ -9679,24 +9653,16 @@
       <c r="G101">
         <v>257</v>
       </c>
-      <c r="H101" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="H101" s="1"/>
       <c r="I101" t="s">
-        <v>354</v>
-      </c>
-      <c r="J101" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>355</v>
+      </c>
+      <c r="J101" s="1"/>
       <c r="K101">
         <v>1</v>
       </c>
-      <c r="L101" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M101" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
       <c r="N101">
         <f>IF(ISERR(FIND(")11",H101))=TRUE,0,1)</f>
         <v>0</v>
@@ -9708,9 +9674,7 @@
         <f>IF(ISERR(FIND(")11",I101))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="Q101" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q101" s="1"/>
       <c r="R101">
         <f>IF(ISERR(FIND(")11",J101))=TRUE,0,1)</f>
         <v>0</v>
@@ -9719,7 +9683,7 @@
         <v>1.3</v>
       </c>
       <c r="T101" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U101">
         <v>0</v>
@@ -9734,13 +9698,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D102" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1">
@@ -9749,24 +9713,16 @@
       <c r="G102">
         <v>258</v>
       </c>
-      <c r="H102" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="H102" s="1"/>
       <c r="I102" t="s">
-        <v>358</v>
-      </c>
-      <c r="J102" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="J102" s="1"/>
       <c r="K102">
         <v>1</v>
       </c>
-      <c r="L102" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M102" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
       <c r="N102">
         <f>IF(ISERR(FIND(")11",H102))=TRUE,0,1)</f>
         <v>0</v>
@@ -9778,9 +9734,7 @@
         <f>IF(ISERR(FIND(")11",I102))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="Q102" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q102" s="1"/>
       <c r="R102">
         <f>IF(ISERR(FIND(")11",J102))=TRUE,0,1)</f>
         <v>0</v>
@@ -9789,7 +9743,7 @@
         <v>1.3</v>
       </c>
       <c r="T102" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U102">
         <v>0</v>
@@ -9804,13 +9758,13 @@
         <v>102</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D103" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1">
@@ -9819,24 +9773,16 @@
       <c r="G103">
         <v>259</v>
       </c>
-      <c r="H103" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="H103" s="1"/>
       <c r="I103" t="s">
-        <v>358</v>
-      </c>
-      <c r="J103" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="J103" s="1"/>
       <c r="K103">
         <v>1</v>
       </c>
-      <c r="L103" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M103" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
       <c r="N103">
         <f>IF(ISERR(FIND(")11",H103))=TRUE,0,1)</f>
         <v>0</v>
@@ -9848,9 +9794,7 @@
         <f>IF(ISERR(FIND(")11",I103))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="Q103" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q103" s="1"/>
       <c r="R103">
         <f>IF(ISERR(FIND(")11",J103))=TRUE,0,1)</f>
         <v>0</v>
@@ -9859,7 +9803,7 @@
         <v>1.3</v>
       </c>
       <c r="T103" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U103">
         <v>0</v>
@@ -9874,13 +9818,13 @@
         <v>103</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D104" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E104" s="1">
         <v>3</v>
@@ -9891,24 +9835,16 @@
       <c r="G104">
         <v>262</v>
       </c>
-      <c r="H104" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="H104" s="1"/>
       <c r="I104" t="s">
-        <v>365</v>
-      </c>
-      <c r="J104" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="J104" s="1"/>
       <c r="K104">
         <v>1</v>
       </c>
-      <c r="L104" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M104" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
       <c r="N104">
         <f>IF(ISERR(FIND(")11",H104))=TRUE,0,1)</f>
         <v>0</v>
@@ -9920,9 +9856,7 @@
         <f>IF(ISERR(FIND(")11",I104))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="Q104" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q104" s="1"/>
       <c r="R104">
         <f>IF(ISERR(FIND(")11",J104))=TRUE,0,1)</f>
         <v>0</v>
@@ -9931,7 +9865,7 @@
         <v>1.3</v>
       </c>
       <c r="T104" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U104">
         <v>0</v>
@@ -9946,13 +9880,13 @@
         <v>104</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D105" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E105" s="1">
         <v>4</v>
@@ -9964,20 +9898,18 @@
         <v>267</v>
       </c>
       <c r="H105" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="I105" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="J105" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="K105">
         <v>1</v>
       </c>
-      <c r="L105" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L105" s="1"/>
       <c r="M105" s="1">
         <v>23.2</v>
       </c>
@@ -9999,11 +9931,9 @@
         <f>IF(ISERR(FIND(")11",J105))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="S105" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S105" s="1"/>
       <c r="T105" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U105">
         <v>0</v>
@@ -10018,13 +9948,13 @@
         <v>105</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D106" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E106" s="1">
         <v>5</v>
@@ -10036,20 +9966,14 @@
         <v>268</v>
       </c>
       <c r="H106" t="s">
-        <v>375</v>
-      </c>
-      <c r="I106" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J106" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>376</v>
+      </c>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
       <c r="K106">
         <v>1</v>
       </c>
-      <c r="L106" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L106" s="1"/>
       <c r="M106" s="1">
         <v>29.3</v>
       </c>
@@ -10057,25 +9981,19 @@
         <f>IF(ISERR(FIND(")11",H106))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="O106" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="O106" s="1"/>
       <c r="P106">
         <f>IF(ISERR(FIND(")11",I106))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="Q106" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q106" s="1"/>
       <c r="R106">
         <f>IF(ISERR(FIND(")11",J106))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S106" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S106" s="1"/>
       <c r="T106" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U106">
         <v>0</v>
@@ -10090,13 +10008,13 @@
         <v>106</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D107" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E107" s="1">
         <v>6</v>
@@ -10108,20 +10026,18 @@
         <v>269</v>
       </c>
       <c r="H107" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K107">
         <v>1</v>
       </c>
-      <c r="L107" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L107" s="1"/>
       <c r="M107" s="1">
         <v>35</v>
       </c>
@@ -10129,25 +10045,19 @@
         <f>IF(ISERR(FIND(")11",H107))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="O107" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="O107" s="1"/>
       <c r="P107">
         <f>IF(ISERR(FIND(")11",I107))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="Q107" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q107" s="1"/>
       <c r="R107">
         <f>IF(ISERR(FIND(")11",J107))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S107" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S107" s="1"/>
       <c r="T107" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U107">
         <v>0</v>
@@ -10162,13 +10072,13 @@
         <v>107</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D108" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E108" s="1">
         <v>7</v>
@@ -10180,20 +10090,18 @@
         <v>270</v>
       </c>
       <c r="H108" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K108">
         <v>1</v>
       </c>
-      <c r="L108" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L108" s="1"/>
       <c r="M108" s="1">
         <v>37.1</v>
       </c>
@@ -10201,25 +10109,19 @@
         <f>IF(ISERR(FIND(")11",H108))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="O108" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="O108" s="1"/>
       <c r="P108">
         <f>IF(ISERR(FIND(")11",I108))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="Q108" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q108" s="1"/>
       <c r="R108">
         <f>IF(ISERR(FIND(")11",J108))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S108" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S108" s="1"/>
       <c r="T108" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U108">
         <v>0</v>
@@ -10234,13 +10136,13 @@
         <v>108</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D109" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E109" s="1">
         <v>8</v>
@@ -10252,20 +10154,18 @@
         <v>269</v>
       </c>
       <c r="H109" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K109">
         <v>1</v>
       </c>
-      <c r="L109" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L109" s="1"/>
       <c r="M109" s="1">
         <v>40.700000000000003</v>
       </c>
@@ -10273,25 +10173,19 @@
         <f>IF(ISERR(FIND(")11",H109))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="O109" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="O109" s="1"/>
       <c r="P109">
         <f>IF(ISERR(FIND(")11",I109))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="Q109" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q109" s="1"/>
       <c r="R109">
         <f>IF(ISERR(FIND(")11",J109))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S109" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S109" s="1"/>
       <c r="T109" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U109">
         <v>0</v>
@@ -10306,13 +10200,13 @@
         <v>109</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D110" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E110" s="1">
         <v>9</v>
@@ -10324,20 +10218,18 @@
         <v>278</v>
       </c>
       <c r="H110" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K110">
         <v>1</v>
       </c>
-      <c r="L110" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L110" s="1"/>
       <c r="M110" s="1">
         <v>37.4</v>
       </c>
@@ -10345,25 +10237,19 @@
         <f>IF(ISERR(FIND(")11",H110))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="O110" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="O110" s="1"/>
       <c r="P110">
         <f>IF(ISERR(FIND(")11",I110))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="Q110" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q110" s="1"/>
       <c r="R110">
         <f>IF(ISERR(FIND(")11",J110))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S110" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S110" s="1"/>
       <c r="T110" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U110">
         <v>0</v>
@@ -10378,13 +10264,13 @@
         <v>110</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D111" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E111" s="1">
         <v>10</v>
@@ -10396,20 +10282,18 @@
         <v>281</v>
       </c>
       <c r="H111" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K111">
         <v>1</v>
       </c>
-      <c r="L111" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L111" s="1"/>
       <c r="M111" s="1">
         <v>34.799999999999997</v>
       </c>
@@ -10417,25 +10301,19 @@
         <f>IF(ISERR(FIND(")11",H111))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="O111" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="O111" s="1"/>
       <c r="P111">
         <f>IF(ISERR(FIND(")11",I111))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="Q111" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q111" s="1"/>
       <c r="R111">
         <f>IF(ISERR(FIND(")11",J111))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S111" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S111" s="1"/>
       <c r="T111" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U111">
         <v>0</v>
@@ -10450,13 +10328,13 @@
         <v>111</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D112" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E112" s="1">
         <v>11</v>
@@ -10468,20 +10346,18 @@
         <v>281</v>
       </c>
       <c r="H112" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K112">
         <v>1</v>
       </c>
-      <c r="L112" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L112" s="1"/>
       <c r="M112" s="1">
         <v>28.7</v>
       </c>
@@ -10489,25 +10365,19 @@
         <f>IF(ISERR(FIND(")11",H112))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="O112" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="O112" s="1"/>
       <c r="P112">
         <f>IF(ISERR(FIND(")11",I112))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="Q112" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q112" s="1"/>
       <c r="R112">
         <f>IF(ISERR(FIND(")11",J112))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S112" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S112" s="1"/>
       <c r="T112" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U112">
         <v>0</v>
@@ -10522,13 +10392,13 @@
         <v>112</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D113" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E113" s="1">
         <v>12</v>
@@ -10540,20 +10410,18 @@
         <v>285</v>
       </c>
       <c r="H113" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J113" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="K113">
         <v>1</v>
       </c>
-      <c r="L113" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L113" s="1"/>
       <c r="M113" s="1">
         <v>23.7</v>
       </c>
@@ -10561,9 +10429,7 @@
         <f>IF(ISERR(FIND(")11",H113))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="O113" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="O113" s="1"/>
       <c r="P113">
         <f>IF(ISERR(FIND(")11",I113))=TRUE,0,1)</f>
         <v>0</v>
@@ -10575,11 +10441,9 @@
         <f>IF(ISERR(FIND(")11",J113))=TRUE,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S113" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S113" s="1"/>
       <c r="T113" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U113">
         <v>0</v>
@@ -10594,13 +10458,13 @@
         <v>113</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E114" s="1">
         <v>13</v>
@@ -10612,20 +10476,18 @@
         <v>286</v>
       </c>
       <c r="H114" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I114" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J114" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K114">
         <v>1</v>
       </c>
-      <c r="L114" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L114" s="1"/>
       <c r="M114" s="1">
         <v>16</v>
       </c>
@@ -10647,11 +10509,9 @@
         <f>IF(ISERR(FIND(")11",J114))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="S114" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S114" s="1"/>
       <c r="T114" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U114">
         <v>0</v>
@@ -10666,13 +10526,13 @@
         <v>114</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D115" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E115" s="1">
         <v>14</v>
@@ -10684,20 +10544,18 @@
         <v>289</v>
       </c>
       <c r="H115" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I115" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="J115" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="K115">
         <v>1</v>
       </c>
-      <c r="L115" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L115" s="1"/>
       <c r="M115" s="1">
         <v>14</v>
       </c>
@@ -10719,11 +10577,9 @@
         <f>IF(ISERR(FIND(")11",J115))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="S115" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S115" s="1"/>
       <c r="T115" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U115">
         <v>0</v>
@@ -10738,13 +10594,13 @@
         <v>115</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E116" s="1">
         <v>15</v>
@@ -10756,20 +10612,18 @@
         <v>288</v>
       </c>
       <c r="H116" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="I116" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J116" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K116">
         <v>1</v>
       </c>
-      <c r="L116" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L116" s="1"/>
       <c r="M116" s="1">
         <v>13.5</v>
       </c>
@@ -10791,11 +10645,9 @@
         <f>IF(ISERR(FIND(")11",J116))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="S116" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S116" s="1"/>
       <c r="T116" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U116">
         <v>0</v>
@@ -10810,13 +10662,13 @@
         <v>116</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E117" s="1">
         <v>16</v>
@@ -10828,20 +10680,18 @@
         <v>293</v>
       </c>
       <c r="H117" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="I117" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="J117" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K117">
         <v>1</v>
       </c>
-      <c r="L117" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L117" s="1"/>
       <c r="M117" s="1">
         <v>12.9</v>
       </c>
@@ -10863,11 +10713,9 @@
         <f>IF(ISERR(FIND(")11",J117))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="S117" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S117" s="1"/>
       <c r="T117" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U117">
         <v>0</v>
@@ -10882,13 +10730,13 @@
         <v>117</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E118" s="1">
         <v>17</v>
@@ -10900,20 +10748,18 @@
         <v>294</v>
       </c>
       <c r="H118" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="I118" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="J118" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="K118">
         <v>1</v>
       </c>
-      <c r="L118" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L118" s="1"/>
       <c r="M118" s="1">
         <v>7.2</v>
       </c>
@@ -10935,11 +10781,9 @@
         <f>IF(ISERR(FIND(")11",J118))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="S118" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S118" s="1"/>
       <c r="T118" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U118">
         <v>0</v>
@@ -10954,13 +10798,13 @@
         <v>118</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E119" s="1">
         <v>18</v>
@@ -10972,20 +10816,18 @@
         <v>294</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="I119" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="J119" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="K119">
         <v>1</v>
       </c>
-      <c r="L119" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="L119" s="1"/>
       <c r="M119" s="1">
         <v>5</v>
       </c>
@@ -11007,11 +10849,9 @@
         <f>IF(ISERR(FIND(")11",J119))=TRUE,0,1)</f>
         <v>1</v>
       </c>
-      <c r="S119" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="S119" s="1"/>
       <c r="T119" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="U119">
         <v>0</v>
@@ -11165,10 +11005,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>